<commit_message>
ipt linked to hiv module, called at ART start
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7314" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7316" uniqueCount="158">
   <si>
     <t>Name:</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>retreatment</t>
+  </si>
+  <si>
+    <t>prop_smear_positive</t>
+  </si>
+  <si>
+    <t>prop_smear_positive_hiv</t>
   </si>
 </sst>
 </file>
@@ -4106,10 +4112,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4387,6 +4393,22 @@
       </c>
       <c r="F23" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4741,7 +4763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
edited FOI for tb susc cases
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -4171,7 +4171,7 @@
         <v>141</v>
       </c>
       <c r="B4">
-        <v>8.3329861207515066E-5</v>
+        <v>4.1579981548900413E-3</v>
       </c>
       <c r="F4" t="s">
         <v>70</v>
@@ -4334,7 +4334,7 @@
         <v>77</v>
       </c>
       <c r="B18">
-        <v>7.4999999999999997E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F18" t="s">
         <v>79</v>
@@ -4422,7 +4422,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4485,15 +4485,15 @@
         <v>148</v>
       </c>
       <c r="B4">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F4">
         <f>B4/12</f>
-        <v>8.3333333333333331E-5</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="G4">
         <f>1-(EXP(-F4))</f>
-        <v>8.3329861207515066E-5</v>
+        <v>4.1579981548900413E-3</v>
       </c>
       <c r="I4" t="s">
         <v>70</v>
@@ -5359,8 +5359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3435"/>
   <sheetViews>
-    <sheetView topLeftCell="A3215" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F3248" sqref="F3248:F3249"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3295" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3248" sqref="F3248:F3249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
active tb onset scheduled hsi sputum tests scheduled as follow-up appts clinical monitoring scheduled after treatment
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="DALY weights" sheetId="17" r:id="rId2"/>
     <sheet name="Structure" sheetId="2" r:id="rId3"/>
     <sheet name="parameters" sheetId="16" r:id="rId4"/>
-    <sheet name="details_rates" sheetId="18" r:id="rId5"/>
-    <sheet name="followup" sheetId="19" r:id="rId6"/>
-    <sheet name="Active_TB_summary" sheetId="4" r:id="rId7"/>
-    <sheet name="Active_TB_prob" sheetId="15" r:id="rId8"/>
-    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId9"/>
-    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId10"/>
-    <sheet name="References" sheetId="7" r:id="rId11"/>
+    <sheet name="pulm_tb" sheetId="20" r:id="rId5"/>
+    <sheet name="details_rates" sheetId="18" r:id="rId6"/>
+    <sheet name="followup" sheetId="19" r:id="rId7"/>
+    <sheet name="Active_TB_summary" sheetId="4" r:id="rId8"/>
+    <sheet name="Active_TB_prob" sheetId="15" r:id="rId9"/>
+    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId10"/>
+    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId11"/>
+    <sheet name="References" sheetId="7" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7316" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7323" uniqueCount="164">
   <si>
     <t>Name:</t>
   </si>
@@ -512,16 +513,34 @@
     <t>abouyannis</t>
   </si>
   <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>retreatment</t>
-  </si>
-  <si>
     <t>prop_smear_positive</t>
   </si>
   <si>
     <t>prop_smear_positive_hiv</t>
+  </si>
+  <si>
+    <t>hiv</t>
+  </si>
+  <si>
+    <t>prob_pulm</t>
+  </si>
+  <si>
+    <t>treatment_clinical</t>
+  </si>
+  <si>
+    <t>treatment_sputum</t>
+  </si>
+  <si>
+    <t>retreatment_clinical</t>
+  </si>
+  <si>
+    <t>retreatment_sputum</t>
+  </si>
+  <si>
+    <t>mdr_clinical</t>
+  </si>
+  <si>
+    <t>mdr_sputum</t>
   </si>
 </sst>
 </file>
@@ -1401,6 +1420,72 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>525000</v>
+      </c>
+      <c r="C2">
+        <v>7847053</v>
+      </c>
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>6.6904097627478745E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <f>3170000-525000</f>
+        <v>2645000</v>
+      </c>
+      <c r="C3">
+        <v>9726553</v>
+      </c>
+      <c r="D3">
+        <f>B3/C3</f>
+        <v>0.27193600857364369</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3696,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4114,7 +4199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -4397,7 +4482,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B24">
         <v>0.8</v>
@@ -4405,7 +4490,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25">
         <v>0.5</v>
@@ -4418,6 +4503,2089 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C188"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="b">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="b">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="b">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="b">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="b">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="b">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="b">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="b">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="b">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="b">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="b">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="b">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="b">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="b">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="b">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="b">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="b">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>15</v>
+      </c>
+      <c r="B103" t="b">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>16</v>
+      </c>
+      <c r="B104" t="b">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>17</v>
+      </c>
+      <c r="B105" t="b">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>18</v>
+      </c>
+      <c r="B106" t="b">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>19</v>
+      </c>
+      <c r="B107" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>20</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>21</v>
+      </c>
+      <c r="B109" t="b">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>22</v>
+      </c>
+      <c r="B110" t="b">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>23</v>
+      </c>
+      <c r="B111" t="b">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>24</v>
+      </c>
+      <c r="B112" t="b">
+        <v>1</v>
+      </c>
+      <c r="C112">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>25</v>
+      </c>
+      <c r="B113" t="b">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>26</v>
+      </c>
+      <c r="B114" t="b">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>27</v>
+      </c>
+      <c r="B115" t="b">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>28</v>
+      </c>
+      <c r="B116" t="b">
+        <v>1</v>
+      </c>
+      <c r="C116">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>29</v>
+      </c>
+      <c r="B117" t="b">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>30</v>
+      </c>
+      <c r="B118" t="b">
+        <v>1</v>
+      </c>
+      <c r="C118">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>31</v>
+      </c>
+      <c r="B119" t="b">
+        <v>1</v>
+      </c>
+      <c r="C119">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>32</v>
+      </c>
+      <c r="B120" t="b">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>33</v>
+      </c>
+      <c r="B121" t="b">
+        <v>1</v>
+      </c>
+      <c r="C121">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>34</v>
+      </c>
+      <c r="B122" t="b">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>35</v>
+      </c>
+      <c r="B123" t="b">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>36</v>
+      </c>
+      <c r="B124" t="b">
+        <v>1</v>
+      </c>
+      <c r="C124">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>37</v>
+      </c>
+      <c r="B125" t="b">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>38</v>
+      </c>
+      <c r="B126" t="b">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>39</v>
+      </c>
+      <c r="B127" t="b">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>40</v>
+      </c>
+      <c r="B128" t="b">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>41</v>
+      </c>
+      <c r="B129" t="b">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>42</v>
+      </c>
+      <c r="B130" t="b">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>43</v>
+      </c>
+      <c r="B131" t="b">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>44</v>
+      </c>
+      <c r="B132" t="b">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>45</v>
+      </c>
+      <c r="B133" t="b">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>46</v>
+      </c>
+      <c r="B134" t="b">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>47</v>
+      </c>
+      <c r="B135" t="b">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>48</v>
+      </c>
+      <c r="B136" t="b">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>49</v>
+      </c>
+      <c r="B137" t="b">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>50</v>
+      </c>
+      <c r="B138" t="b">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>51</v>
+      </c>
+      <c r="B139" t="b">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>52</v>
+      </c>
+      <c r="B140" t="b">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>53</v>
+      </c>
+      <c r="B141" t="b">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>54</v>
+      </c>
+      <c r="B142" t="b">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>55</v>
+      </c>
+      <c r="B143" t="b">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>56</v>
+      </c>
+      <c r="B144" t="b">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>57</v>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>58</v>
+      </c>
+      <c r="B146" t="b">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>59</v>
+      </c>
+      <c r="B147" t="b">
+        <v>1</v>
+      </c>
+      <c r="C147">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>60</v>
+      </c>
+      <c r="B148" t="b">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>61</v>
+      </c>
+      <c r="B149" t="b">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>62</v>
+      </c>
+      <c r="B150" t="b">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>63</v>
+      </c>
+      <c r="B151" t="b">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>64</v>
+      </c>
+      <c r="B152" t="b">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>65</v>
+      </c>
+      <c r="B153" t="b">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>66</v>
+      </c>
+      <c r="B154" t="b">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>67</v>
+      </c>
+      <c r="B155" t="b">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>68</v>
+      </c>
+      <c r="B156" t="b">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>69</v>
+      </c>
+      <c r="B157" t="b">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>70</v>
+      </c>
+      <c r="B158" t="b">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>71</v>
+      </c>
+      <c r="B159" t="b">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>72</v>
+      </c>
+      <c r="B160" t="b">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>73</v>
+      </c>
+      <c r="B161" t="b">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>74</v>
+      </c>
+      <c r="B162" t="b">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>75</v>
+      </c>
+      <c r="B163" t="b">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>76</v>
+      </c>
+      <c r="B164" t="b">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>77</v>
+      </c>
+      <c r="B165" t="b">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>78</v>
+      </c>
+      <c r="B166" t="b">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>79</v>
+      </c>
+      <c r="B167" t="b">
+        <v>1</v>
+      </c>
+      <c r="C167">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>80</v>
+      </c>
+      <c r="B168" t="b">
+        <v>1</v>
+      </c>
+      <c r="C168">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>81</v>
+      </c>
+      <c r="B169" t="b">
+        <v>1</v>
+      </c>
+      <c r="C169">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>82</v>
+      </c>
+      <c r="B170" t="b">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>83</v>
+      </c>
+      <c r="B171" t="b">
+        <v>1</v>
+      </c>
+      <c r="C171">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>84</v>
+      </c>
+      <c r="B172" t="b">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>85</v>
+      </c>
+      <c r="B173" t="b">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>86</v>
+      </c>
+      <c r="B174" t="b">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>87</v>
+      </c>
+      <c r="B175" t="b">
+        <v>1</v>
+      </c>
+      <c r="C175">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>88</v>
+      </c>
+      <c r="B176" t="b">
+        <v>1</v>
+      </c>
+      <c r="C176">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>89</v>
+      </c>
+      <c r="B177" t="b">
+        <v>1</v>
+      </c>
+      <c r="C177">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>90</v>
+      </c>
+      <c r="B178" t="b">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>91</v>
+      </c>
+      <c r="B179" t="b">
+        <v>1</v>
+      </c>
+      <c r="C179">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>92</v>
+      </c>
+      <c r="B180" t="b">
+        <v>1</v>
+      </c>
+      <c r="C180">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>93</v>
+      </c>
+      <c r="B181" t="b">
+        <v>1</v>
+      </c>
+      <c r="C181">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>94</v>
+      </c>
+      <c r="B182" t="b">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>95</v>
+      </c>
+      <c r="B183" t="b">
+        <v>1</v>
+      </c>
+      <c r="C183">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>96</v>
+      </c>
+      <c r="B184" t="b">
+        <v>1</v>
+      </c>
+      <c r="C184">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>97</v>
+      </c>
+      <c r="B185" t="b">
+        <v>1</v>
+      </c>
+      <c r="C185">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>98</v>
+      </c>
+      <c r="B186" t="b">
+        <v>1</v>
+      </c>
+      <c r="C186">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>99</v>
+      </c>
+      <c r="B187" t="b">
+        <v>1</v>
+      </c>
+      <c r="C187">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>100</v>
+      </c>
+      <c r="B188" t="b">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -4759,83 +6927,241 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="E8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9">
         <v>28</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4843,7 +7169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -5355,7 +7681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3435"/>
   <sheetViews>
@@ -73467,70 +75793,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2">
-        <v>525000</v>
-      </c>
-      <c r="C2">
-        <v>7847053</v>
-      </c>
-      <c r="D2">
-        <f>B2/C2</f>
-        <v>6.6904097627478745E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <f>3170000-525000</f>
-        <v>2645000</v>
-      </c>
-      <c r="C3">
-        <v>9726553</v>
-      </c>
-      <c r="D3">
-        <f>B3/C3</f>
-        <v>0.27193600857364369</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
tb on_his_alert linked to hiv testing and treatment
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7529" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7534" uniqueCount="205">
   <si>
     <t>Name:</t>
   </si>
@@ -475,9 +475,6 @@
     <t>tb_mortality_hiv_rate</t>
   </si>
   <si>
-    <t>monthly_prob_progr_active</t>
-  </si>
-  <si>
     <t>monthly_prob_relapse_tx_complete</t>
   </si>
   <si>
@@ -508,16 +505,10 @@
     <t>monthly_prob_tb_mortality_hiv</t>
   </si>
   <si>
-    <t>prob_treatment_success</t>
-  </si>
-  <si>
     <t>abouyannis</t>
   </si>
   <si>
     <t>prop_smear_positive</t>
-  </si>
-  <si>
-    <t>prop_smear_positive_hiv</t>
   </si>
   <si>
     <t>hiv</t>
@@ -546,12 +537,141 @@
   <si>
     <t>Proportion_pop_with_active_tb</t>
   </si>
+  <si>
+    <t>prop_latent_child_2010</t>
+  </si>
+  <si>
+    <t>prop_latent_adult_2010</t>
+  </si>
+  <si>
+    <t>prop_active_2010</t>
+  </si>
+  <si>
+    <t>rel_inf_hiv</t>
+  </si>
+  <si>
+    <t>rel_inf_smear_ng</t>
+  </si>
+  <si>
+    <t>rr_bcg_inf</t>
+  </si>
+  <si>
+    <t>prog_active</t>
+  </si>
+  <si>
+    <t>progr_1yr</t>
+  </si>
+  <si>
+    <t>progr_1_2yr</t>
+  </si>
+  <si>
+    <t>progr2_5yr</t>
+  </si>
+  <si>
+    <t>progr5_10yr</t>
+  </si>
+  <si>
+    <t>progr_10yr</t>
+  </si>
+  <si>
+    <t>prop_pulm</t>
+  </si>
+  <si>
+    <t>prop_pulm_hiv</t>
+  </si>
+  <si>
+    <t>prop_pulm_1yr</t>
+  </si>
+  <si>
+    <t>prop_pulm_1_2yr</t>
+  </si>
+  <si>
+    <t>prop_pulm_2_5yr</t>
+  </si>
+  <si>
+    <t>prop_pulm_5_10yr</t>
+  </si>
+  <si>
+    <t>prop_pulm_10yr</t>
+  </si>
+  <si>
+    <t>mortality_cotrim</t>
+  </si>
+  <si>
+    <t>rr_tb_bcg</t>
+  </si>
+  <si>
+    <t>rr_tb_hiv</t>
+  </si>
+  <si>
+    <t>rr_tb_art_adult</t>
+  </si>
+  <si>
+    <t>rr_tb_art_child</t>
+  </si>
+  <si>
+    <t>rr_tb_overweight</t>
+  </si>
+  <si>
+    <t>rr_tb_obese</t>
+  </si>
+  <si>
+    <t>dur_prot_ipt</t>
+  </si>
+  <si>
+    <t>dur_prot_ipt_infant</t>
+  </si>
+  <si>
+    <t>rr_ipt_adult</t>
+  </si>
+  <si>
+    <t>rr_ipt_child</t>
+  </si>
+  <si>
+    <t>rr_ipt_adult_hiv</t>
+  </si>
+  <si>
+    <t>rr_ipt_child_hiv</t>
+  </si>
+  <si>
+    <t>rr_ipt_art_child</t>
+  </si>
+  <si>
+    <t>rr_ipt_art_adult</t>
+  </si>
+  <si>
+    <t>prop_fail_xpert</t>
+  </si>
+  <si>
+    <t>prob_tx_success_new</t>
+  </si>
+  <si>
+    <t>prob_tx_success_prev</t>
+  </si>
+  <si>
+    <t>prob_tx_success_hiv</t>
+  </si>
+  <si>
+    <t>prob_tx_success_mdr</t>
+  </si>
+  <si>
+    <t>prob_tx_success_extra</t>
+  </si>
+  <si>
+    <t>prob_tx_success_0_14</t>
+  </si>
+  <si>
+    <t>prob_tx_success_5_14</t>
+  </si>
+  <si>
+    <t>transmission rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -587,6 +707,44 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -614,7 +772,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -745,11 +903,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCBD2DC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCBD2DC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCBD2DC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFB2BBCB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCBD2DC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCBD2DC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCBD2DC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -805,6 +991,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -72315,10 +72525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A21:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -72327,291 +72537,452 @@
     <col min="2" max="2" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="29">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="27">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="27">
+        <v>3.3E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="30">
+        <v>1.8599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="30">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="30">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="30">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="30">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="30">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B2">
+      <c r="B13" s="30">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3">
-        <v>1E-3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4">
-        <v>4.1579981548900413E-3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5">
-        <v>3.44</v>
-      </c>
-      <c r="C5">
-        <v>6.76</v>
-      </c>
-      <c r="D5">
-        <v>13.28</v>
-      </c>
-      <c r="E5">
-        <v>26.06</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6">
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="30">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="30">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="30">
+        <v>1.6500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="30">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="30">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="30">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="30">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="30">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="30">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="30">
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="30">
+        <v>6.7699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="30">
         <v>0.35</v>
       </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7">
+    </row>
+    <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="27">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="27">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="27">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="31">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="30">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="30">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" s="27">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" s="27">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="27">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="27">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="27">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B47" s="27">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" s="27">
         <v>0.63</v>
       </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8">
-        <v>2.1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10">
-        <v>2.9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11">
-        <v>2.6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12">
-        <v>1.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13">
-        <v>0.68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14">
-        <v>1.6528546178382508E-2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15">
-        <v>1.2422199506118559E-2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16">
-        <v>6.7606180094051727E-2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17">
-        <v>1.8599999999999998E-2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20">
-        <v>2.6631142694990562E-3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21">
-        <v>1.1598875001476161E-2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22">
-        <v>1.2499218782546784E-4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23">
-        <v>0.86</v>
-      </c>
-      <c r="F23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>154</v>
-      </c>
-      <c r="B24">
+    </row>
+    <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" s="27">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="27">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="27">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="27">
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25">
-        <v>0.5</v>
+    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="27">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="27">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="27">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="27">
+        <v>0.84399999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -72635,10 +73006,10 @@
         <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -74768,7 +75139,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4">
         <v>0.05</v>
@@ -74895,7 +75266,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14">
         <v>0.2</v>
@@ -74909,7 +75280,7 @@
         <v>1.6528546178382508E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -74958,7 +75329,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="I17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -75065,22 +75436,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" t="s">
         <v>158</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -75327,7 +75698,7 @@
         <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -75803,7 +76174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D168" sqref="D168:D203"/>
     </sheetView>
   </sheetViews>
@@ -75823,7 +76194,7 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
backup checks if xpert not available, give sputum smear
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7534" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7534" uniqueCount="204">
   <si>
     <t>Name:</t>
   </si>
@@ -565,12 +565,6 @@
     <t>progr_1_2yr</t>
   </si>
   <si>
-    <t>progr2_5yr</t>
-  </si>
-  <si>
-    <t>progr5_10yr</t>
-  </si>
-  <si>
     <t>progr_10yr</t>
   </si>
   <si>
@@ -664,7 +658,10 @@
     <t>prob_tx_success_5_14</t>
   </si>
   <si>
-    <t>transmission rate</t>
+    <t>progr_2_5yr</t>
+  </si>
+  <si>
+    <t>progr_5_10yr</t>
   </si>
 </sst>
 </file>
@@ -72527,8 +72524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A27" sqref="A21:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -72579,7 +72576,7 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>204</v>
+        <v>69</v>
       </c>
       <c r="B6" s="27">
         <v>0.5</v>
@@ -72667,7 +72664,7 @@
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="B17" s="30">
         <v>0.05</v>
@@ -72675,7 +72672,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="B18" s="30">
         <v>0.02</v>
@@ -72683,7 +72680,7 @@
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B19" s="30">
         <v>0.15</v>
@@ -72699,7 +72696,7 @@
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B21" s="30">
         <v>0.8</v>
@@ -72707,7 +72704,7 @@
     </row>
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B22" s="30">
         <v>0.5</v>
@@ -72715,7 +72712,7 @@
     </row>
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23" s="30">
         <v>0.7</v>
@@ -72723,7 +72720,7 @@
     </row>
     <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B24" s="30">
         <v>0.74</v>
@@ -72731,7 +72728,7 @@
     </row>
     <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" s="30">
         <v>0.91</v>
@@ -72739,7 +72736,7 @@
     </row>
     <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B26" s="30">
         <v>0.89</v>
@@ -72747,7 +72744,7 @@
     </row>
     <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B27" s="30">
         <v>0.99</v>
@@ -72779,7 +72776,7 @@
     </row>
     <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B31" s="30">
         <v>0.35</v>
@@ -72787,7 +72784,7 @@
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B32" s="27">
         <v>0.42</v>
@@ -72795,7 +72792,7 @@
     </row>
     <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B33" s="27">
         <v>5</v>
@@ -72803,7 +72800,7 @@
     </row>
     <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B34" s="27">
         <v>0.35</v>
@@ -72811,7 +72808,7 @@
     </row>
     <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B35" s="27">
         <v>0.3</v>
@@ -72819,7 +72816,7 @@
     </row>
     <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B36" s="31">
         <v>0.62</v>
@@ -72827,7 +72824,7 @@
     </row>
     <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B37" s="31">
         <v>0.4</v>
@@ -72859,7 +72856,7 @@
     </row>
     <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B41" s="27">
         <v>365</v>
@@ -72867,7 +72864,7 @@
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B42" s="27">
         <v>548</v>
@@ -72875,7 +72872,7 @@
     </row>
     <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B43" s="27">
         <v>0.4</v>
@@ -72883,7 +72880,7 @@
     </row>
     <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B44" s="27">
         <v>0.55000000000000004</v>
@@ -72891,7 +72888,7 @@
     </row>
     <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B45" s="27">
         <v>0.68</v>
@@ -72899,7 +72896,7 @@
     </row>
     <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B46" s="27">
         <v>0.86</v>
@@ -72907,7 +72904,7 @@
     </row>
     <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B47" s="27">
         <v>0.76</v>
@@ -72915,7 +72912,7 @@
     </row>
     <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B48" s="27">
         <v>0.63</v>
@@ -72923,7 +72920,7 @@
     </row>
     <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B49" s="27">
         <v>0.15</v>
@@ -72931,7 +72928,7 @@
     </row>
     <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B50" s="27">
         <v>0.82</v>
@@ -72939,7 +72936,7 @@
     </row>
     <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B51" s="27">
         <v>0.81</v>
@@ -72947,7 +72944,7 @@
     </row>
     <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B52" s="27">
         <v>0.8</v>
@@ -72955,7 +72952,7 @@
     </row>
     <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B53" s="27">
         <v>0.61</v>
@@ -72963,7 +72960,7 @@
     </row>
     <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B54" s="27">
         <v>0.78500000000000003</v>
@@ -72971,7 +72968,7 @@
     </row>
     <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B55" s="27">
         <v>0.78200000000000003</v>
@@ -72979,7 +72976,7 @@
     </row>
     <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B56" s="27">
         <v>0.84399999999999997</v>
@@ -76175,7 +76172,7 @@
   <dimension ref="A1:D203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D168" sqref="D168:D203"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
baseline tb cases - scatter active disease onset across 2010
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -655,9 +655,6 @@
     <t>prob_tx_success_extra</t>
   </si>
   <si>
-    <t>prob_tx_success_0_14</t>
-  </si>
-  <si>
     <t>prob_tx_success_5_14</t>
   </si>
   <si>
@@ -665,6 +662,9 @@
   </si>
   <si>
     <t>progr_5_10yr</t>
+  </si>
+  <si>
+    <t>prob_tx_success_0_4</t>
   </si>
 </sst>
 </file>
@@ -986,12 +986,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1015,6 +1009,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -72168,12 +72168,12 @@
   <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -72527,8 +72527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -72546,450 +72546,450 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="27">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="25">
         <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="25">
         <v>3.3E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="28">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="28">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="28">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="28">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="30">
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="28">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="28">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="28">
+        <v>1.6500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="28">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="28">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="28">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="28">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="28">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="28">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="28">
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="28">
+        <v>6.7699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="28">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="25">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" s="29">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="28">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="28">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" s="25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="25">
         <v>0.68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="30">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="30">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="30">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="30">
-        <v>1.1599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="30">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="30">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B16" s="30">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="B17" s="30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+    <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="25">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" s="25">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" s="25">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" s="25">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B53" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" s="25">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="25">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="B18" s="30">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="B19" s="30">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B20" s="30">
-        <v>1.6500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" s="30">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="B22" s="30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="30">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="B24" s="30">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="B25" s="30">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="B26" s="30">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B27" s="30">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="30">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" s="30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B30" s="30">
-        <v>1.24E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="30">
-        <v>6.7699999999999996E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B32" s="30">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="B33" s="27">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="27">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B36" s="27">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="B37" s="31">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="B38" s="31">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="30">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="30">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B42" s="27">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B43" s="27">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="B44" s="27">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" s="27">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="B46" s="27">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="B47" s="27">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="B48" s="27">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B49" s="27">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="B50" s="27">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="B51" s="27">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="B52" s="27">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B53" s="27">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="B54" s="27">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="B55" s="27">
-        <v>0.78500000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="25" t="s">
+      <c r="B56" s="25">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="B56" s="27">
-        <v>0.78200000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="B57" s="27">
+      <c r="B57" s="25">
         <v>0.84399999999999997</v>
       </c>
     </row>
@@ -75671,7 +75671,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small changes - tx duration, relapse rates, self-cure
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="followup" sheetId="19" r:id="rId7"/>
     <sheet name="Active_TB_summary" sheetId="4" r:id="rId8"/>
     <sheet name="ProportionActiveTb" sheetId="21" r:id="rId9"/>
-    <sheet name="Active_TB_prob" sheetId="15" r:id="rId10"/>
-    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId11"/>
-    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId12"/>
-    <sheet name="References" sheetId="7" r:id="rId13"/>
+    <sheet name="PropActive2010Updated" sheetId="22" r:id="rId10"/>
+    <sheet name="Active_TB_prob" sheetId="15" r:id="rId11"/>
+    <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId12"/>
+    <sheet name="Latent_TB_prob" sheetId="13" r:id="rId13"/>
+    <sheet name="References" sheetId="7" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7535" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="209">
   <si>
     <t>Name:</t>
   </si>
@@ -550,9 +551,6 @@
     <t>prop_active_2010</t>
   </si>
   <si>
-    <t>rel_inf_hiv</t>
-  </si>
-  <si>
     <t>rel_inf_smear_ng</t>
   </si>
   <si>
@@ -665,6 +663,21 @@
   </si>
   <si>
     <t>prob_tx_success_0_4</t>
+  </si>
+  <si>
+    <t>prob_active_tb</t>
+  </si>
+  <si>
+    <t>treatment_extrapulm</t>
+  </si>
+  <si>
+    <t>retreatment_extrapulm</t>
+  </si>
+  <si>
+    <t>rr_relapse_hiv</t>
+  </si>
+  <si>
+    <t>monthly_prob_self_cure_hiv</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1647,2867 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D203"/>
+  <sheetViews>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>2010</v>
+      </c>
+      <c r="D2">
+        <v>8.8279781195108931E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="D3">
+        <v>8.8279781195108931E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>2010</v>
+      </c>
+      <c r="D4">
+        <v>8.8279781195108931E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>2010</v>
+      </c>
+      <c r="D5">
+        <v>8.8279781195108931E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>2010</v>
+      </c>
+      <c r="D6">
+        <v>8.8279781195108931E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>2010</v>
+      </c>
+      <c r="D7">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>2010</v>
+      </c>
+      <c r="D8">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>2010</v>
+      </c>
+      <c r="D9">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>2010</v>
+      </c>
+      <c r="D10">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>2010</v>
+      </c>
+      <c r="D12">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
+        <v>2010</v>
+      </c>
+      <c r="D13">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>2010</v>
+      </c>
+      <c r="D14">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>2010</v>
+      </c>
+      <c r="D15">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>2010</v>
+      </c>
+      <c r="D16">
+        <v>3.8184750379774359E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>2010</v>
+      </c>
+      <c r="D17">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>2010</v>
+      </c>
+      <c r="D18">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>2010</v>
+      </c>
+      <c r="D19">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>2010</v>
+      </c>
+      <c r="D20">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>2010</v>
+      </c>
+      <c r="D21">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>2010</v>
+      </c>
+      <c r="D22">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23">
+        <v>2010</v>
+      </c>
+      <c r="D23">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>2010</v>
+      </c>
+      <c r="D24">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25">
+        <v>2010</v>
+      </c>
+      <c r="D25">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>2010</v>
+      </c>
+      <c r="D26">
+        <v>2.0663286458646479E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27">
+        <v>2010</v>
+      </c>
+      <c r="D27">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>2010</v>
+      </c>
+      <c r="D28">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29">
+        <v>2010</v>
+      </c>
+      <c r="D29">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>2010</v>
+      </c>
+      <c r="D30">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31">
+        <v>2010</v>
+      </c>
+      <c r="D31">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32">
+        <v>2010</v>
+      </c>
+      <c r="D32">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>2010</v>
+      </c>
+      <c r="D33">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34">
+        <v>2010</v>
+      </c>
+      <c r="D34">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>2010</v>
+      </c>
+      <c r="D35">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36">
+        <v>2010</v>
+      </c>
+      <c r="D36">
+        <v>7.0375266077884902E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37">
+        <v>2010</v>
+      </c>
+      <c r="D37">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>2010</v>
+      </c>
+      <c r="D38">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39">
+        <v>2010</v>
+      </c>
+      <c r="D39">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
+        <v>2010</v>
+      </c>
+      <c r="D40">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41">
+        <v>2010</v>
+      </c>
+      <c r="D41">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>2010</v>
+      </c>
+      <c r="D42">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>2010</v>
+      </c>
+      <c r="D43">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <v>2010</v>
+      </c>
+      <c r="D44">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>2010</v>
+      </c>
+      <c r="D45">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>2010</v>
+      </c>
+      <c r="D46">
+        <v>1.1856946189270011E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>2010</v>
+      </c>
+      <c r="D47">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48">
+        <v>2010</v>
+      </c>
+      <c r="D48">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>2010</v>
+      </c>
+      <c r="D49">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50">
+        <v>2010</v>
+      </c>
+      <c r="D50">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51">
+        <v>2010</v>
+      </c>
+      <c r="D51">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <v>2010</v>
+      </c>
+      <c r="D52">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53">
+        <v>2010</v>
+      </c>
+      <c r="D53">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54">
+        <v>2010</v>
+      </c>
+      <c r="D54">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55">
+        <v>2010</v>
+      </c>
+      <c r="D55">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56">
+        <v>2010</v>
+      </c>
+      <c r="D56">
+        <v>9.8485521688103407E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57">
+        <v>2010</v>
+      </c>
+      <c r="D57">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58">
+        <v>2010</v>
+      </c>
+      <c r="D58">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59">
+        <v>2010</v>
+      </c>
+      <c r="D59">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60">
+        <v>2010</v>
+      </c>
+      <c r="D60">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61">
+        <v>2010</v>
+      </c>
+      <c r="D61">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62">
+        <v>2010</v>
+      </c>
+      <c r="D62">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63">
+        <v>2010</v>
+      </c>
+      <c r="D63">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64">
+        <v>2010</v>
+      </c>
+      <c r="D64">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65">
+        <v>2010</v>
+      </c>
+      <c r="D65">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66">
+        <v>2010</v>
+      </c>
+      <c r="D66">
+        <v>1.0643670290653847E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67">
+        <v>2010</v>
+      </c>
+      <c r="D67">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68">
+        <v>2010</v>
+      </c>
+      <c r="D68">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69">
+        <v>2010</v>
+      </c>
+      <c r="D69">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70">
+        <v>2010</v>
+      </c>
+      <c r="D70">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71">
+        <v>2010</v>
+      </c>
+      <c r="D71">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72">
+        <v>2010</v>
+      </c>
+      <c r="D72">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73">
+        <v>2010</v>
+      </c>
+      <c r="D73">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74">
+        <v>2010</v>
+      </c>
+      <c r="D74">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75">
+        <v>2010</v>
+      </c>
+      <c r="D75">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76">
+        <v>2010</v>
+      </c>
+      <c r="D76">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77">
+        <v>2010</v>
+      </c>
+      <c r="D77">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>44</v>
+      </c>
+      <c r="C78">
+        <v>2010</v>
+      </c>
+      <c r="D78">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79">
+        <v>2010</v>
+      </c>
+      <c r="D79">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80">
+        <v>2010</v>
+      </c>
+      <c r="D80">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>44</v>
+      </c>
+      <c r="C81">
+        <v>2010</v>
+      </c>
+      <c r="D81">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82">
+        <v>2010</v>
+      </c>
+      <c r="D82">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83">
+        <v>2010</v>
+      </c>
+      <c r="D83">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84">
+        <v>2010</v>
+      </c>
+      <c r="D84">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85">
+        <v>2010</v>
+      </c>
+      <c r="D85">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86">
+        <v>2010</v>
+      </c>
+      <c r="D86">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87">
+        <v>2010</v>
+      </c>
+      <c r="D87">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88">
+        <v>2010</v>
+      </c>
+      <c r="D88">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89">
+        <v>2010</v>
+      </c>
+      <c r="D89">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90">
+        <v>2010</v>
+      </c>
+      <c r="D90">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91">
+        <v>2010</v>
+      </c>
+      <c r="D91">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92">
+        <v>2010</v>
+      </c>
+      <c r="D92">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93">
+        <v>2010</v>
+      </c>
+      <c r="D93">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94">
+        <v>2010</v>
+      </c>
+      <c r="D94">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95">
+        <v>2010</v>
+      </c>
+      <c r="D95">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96">
+        <v>2010</v>
+      </c>
+      <c r="D96">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97">
+        <v>2010</v>
+      </c>
+      <c r="D97">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98">
+        <v>2010</v>
+      </c>
+      <c r="D98">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99">
+        <v>2010</v>
+      </c>
+      <c r="D99">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100">
+        <v>2010</v>
+      </c>
+      <c r="D100">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>44</v>
+      </c>
+      <c r="C101">
+        <v>2010</v>
+      </c>
+      <c r="D101">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>44</v>
+      </c>
+      <c r="C102">
+        <v>2010</v>
+      </c>
+      <c r="D102">
+        <v>1.7037361097110303E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103">
+        <v>2010</v>
+      </c>
+      <c r="D103">
+        <v>7.2937550802143784E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104">
+        <v>2010</v>
+      </c>
+      <c r="D104">
+        <v>7.2937550802143784E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105">
+        <v>2010</v>
+      </c>
+      <c r="D105">
+        <v>7.2937550802143784E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106">
+        <v>2010</v>
+      </c>
+      <c r="D106">
+        <v>7.2937550802143784E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>4</v>
+      </c>
+      <c r="B107" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107">
+        <v>2010</v>
+      </c>
+      <c r="D107">
+        <v>7.2937550802143784E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>41</v>
+      </c>
+      <c r="C108">
+        <v>2010</v>
+      </c>
+      <c r="D108">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>6</v>
+      </c>
+      <c r="B109" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109">
+        <v>2010</v>
+      </c>
+      <c r="D109">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>7</v>
+      </c>
+      <c r="B110" t="s">
+        <v>41</v>
+      </c>
+      <c r="C110">
+        <v>2010</v>
+      </c>
+      <c r="D110">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>8</v>
+      </c>
+      <c r="B111" t="s">
+        <v>41</v>
+      </c>
+      <c r="C111">
+        <v>2010</v>
+      </c>
+      <c r="D111">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>41</v>
+      </c>
+      <c r="C112">
+        <v>2010</v>
+      </c>
+      <c r="D112">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>10</v>
+      </c>
+      <c r="B113" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113">
+        <v>2010</v>
+      </c>
+      <c r="D113">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>11</v>
+      </c>
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114">
+        <v>2010</v>
+      </c>
+      <c r="D114">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s">
+        <v>41</v>
+      </c>
+      <c r="C115">
+        <v>2010</v>
+      </c>
+      <c r="D115">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>13</v>
+      </c>
+      <c r="B116" t="s">
+        <v>41</v>
+      </c>
+      <c r="C116">
+        <v>2010</v>
+      </c>
+      <c r="D116">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>14</v>
+      </c>
+      <c r="B117" t="s">
+        <v>41</v>
+      </c>
+      <c r="C117">
+        <v>2010</v>
+      </c>
+      <c r="D117">
+        <v>3.8369722306016421E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>15</v>
+      </c>
+      <c r="B118" t="s">
+        <v>41</v>
+      </c>
+      <c r="C118">
+        <v>2010</v>
+      </c>
+      <c r="D118">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>16</v>
+      </c>
+      <c r="B119" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119">
+        <v>2010</v>
+      </c>
+      <c r="D119">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>17</v>
+      </c>
+      <c r="B120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C120">
+        <v>2010</v>
+      </c>
+      <c r="D120">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>18</v>
+      </c>
+      <c r="B121" t="s">
+        <v>41</v>
+      </c>
+      <c r="C121">
+        <v>2010</v>
+      </c>
+      <c r="D121">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>19</v>
+      </c>
+      <c r="B122" t="s">
+        <v>41</v>
+      </c>
+      <c r="C122">
+        <v>2010</v>
+      </c>
+      <c r="D122">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>20</v>
+      </c>
+      <c r="B123" t="s">
+        <v>41</v>
+      </c>
+      <c r="C123">
+        <v>2010</v>
+      </c>
+      <c r="D123">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>21</v>
+      </c>
+      <c r="B124" t="s">
+        <v>41</v>
+      </c>
+      <c r="C124">
+        <v>2010</v>
+      </c>
+      <c r="D124">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>22</v>
+      </c>
+      <c r="B125" t="s">
+        <v>41</v>
+      </c>
+      <c r="C125">
+        <v>2010</v>
+      </c>
+      <c r="D125">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>23</v>
+      </c>
+      <c r="B126" t="s">
+        <v>41</v>
+      </c>
+      <c r="C126">
+        <v>2010</v>
+      </c>
+      <c r="D126">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>24</v>
+      </c>
+      <c r="B127" t="s">
+        <v>41</v>
+      </c>
+      <c r="C127">
+        <v>2010</v>
+      </c>
+      <c r="D127">
+        <v>1.4109346418356254E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>25</v>
+      </c>
+      <c r="B128" t="s">
+        <v>41</v>
+      </c>
+      <c r="C128">
+        <v>2010</v>
+      </c>
+      <c r="D128">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>26</v>
+      </c>
+      <c r="B129" t="s">
+        <v>41</v>
+      </c>
+      <c r="C129">
+        <v>2010</v>
+      </c>
+      <c r="D129">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>27</v>
+      </c>
+      <c r="B130" t="s">
+        <v>41</v>
+      </c>
+      <c r="C130">
+        <v>2010</v>
+      </c>
+      <c r="D130">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>28</v>
+      </c>
+      <c r="B131" t="s">
+        <v>41</v>
+      </c>
+      <c r="C131">
+        <v>2010</v>
+      </c>
+      <c r="D131">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>29</v>
+      </c>
+      <c r="B132" t="s">
+        <v>41</v>
+      </c>
+      <c r="C132">
+        <v>2010</v>
+      </c>
+      <c r="D132">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>30</v>
+      </c>
+      <c r="B133" t="s">
+        <v>41</v>
+      </c>
+      <c r="C133">
+        <v>2010</v>
+      </c>
+      <c r="D133">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>31</v>
+      </c>
+      <c r="B134" t="s">
+        <v>41</v>
+      </c>
+      <c r="C134">
+        <v>2010</v>
+      </c>
+      <c r="D134">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>32</v>
+      </c>
+      <c r="B135" t="s">
+        <v>41</v>
+      </c>
+      <c r="C135">
+        <v>2010</v>
+      </c>
+      <c r="D135">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>33</v>
+      </c>
+      <c r="B136" t="s">
+        <v>41</v>
+      </c>
+      <c r="C136">
+        <v>2010</v>
+      </c>
+      <c r="D136">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>34</v>
+      </c>
+      <c r="B137" t="s">
+        <v>41</v>
+      </c>
+      <c r="C137">
+        <v>2010</v>
+      </c>
+      <c r="D137">
+        <v>4.7297010103780034E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>35</v>
+      </c>
+      <c r="B138" t="s">
+        <v>41</v>
+      </c>
+      <c r="C138">
+        <v>2010</v>
+      </c>
+      <c r="D138">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>36</v>
+      </c>
+      <c r="B139" t="s">
+        <v>41</v>
+      </c>
+      <c r="C139">
+        <v>2010</v>
+      </c>
+      <c r="D139">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>37</v>
+      </c>
+      <c r="B140" t="s">
+        <v>41</v>
+      </c>
+      <c r="C140">
+        <v>2010</v>
+      </c>
+      <c r="D140">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>38</v>
+      </c>
+      <c r="B141" t="s">
+        <v>41</v>
+      </c>
+      <c r="C141">
+        <v>2010</v>
+      </c>
+      <c r="D141">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>39</v>
+      </c>
+      <c r="B142" t="s">
+        <v>41</v>
+      </c>
+      <c r="C142">
+        <v>2010</v>
+      </c>
+      <c r="D142">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>40</v>
+      </c>
+      <c r="B143" t="s">
+        <v>41</v>
+      </c>
+      <c r="C143">
+        <v>2010</v>
+      </c>
+      <c r="D143">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>41</v>
+      </c>
+      <c r="B144" t="s">
+        <v>41</v>
+      </c>
+      <c r="C144">
+        <v>2010</v>
+      </c>
+      <c r="D144">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>42</v>
+      </c>
+      <c r="B145" t="s">
+        <v>41</v>
+      </c>
+      <c r="C145">
+        <v>2010</v>
+      </c>
+      <c r="D145">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>43</v>
+      </c>
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146">
+        <v>2010</v>
+      </c>
+      <c r="D146">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>44</v>
+      </c>
+      <c r="B147" t="s">
+        <v>41</v>
+      </c>
+      <c r="C147">
+        <v>2010</v>
+      </c>
+      <c r="D147">
+        <v>7.8340418299316355E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>45</v>
+      </c>
+      <c r="B148" t="s">
+        <v>41</v>
+      </c>
+      <c r="C148">
+        <v>2010</v>
+      </c>
+      <c r="D148">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>46</v>
+      </c>
+      <c r="B149" t="s">
+        <v>41</v>
+      </c>
+      <c r="C149">
+        <v>2010</v>
+      </c>
+      <c r="D149">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>47</v>
+      </c>
+      <c r="B150" t="s">
+        <v>41</v>
+      </c>
+      <c r="C150">
+        <v>2010</v>
+      </c>
+      <c r="D150">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>48</v>
+      </c>
+      <c r="B151" t="s">
+        <v>41</v>
+      </c>
+      <c r="C151">
+        <v>2010</v>
+      </c>
+      <c r="D151">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>49</v>
+      </c>
+      <c r="B152" t="s">
+        <v>41</v>
+      </c>
+      <c r="C152">
+        <v>2010</v>
+      </c>
+      <c r="D152">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>50</v>
+      </c>
+      <c r="B153" t="s">
+        <v>41</v>
+      </c>
+      <c r="C153">
+        <v>2010</v>
+      </c>
+      <c r="D153">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>51</v>
+      </c>
+      <c r="B154" t="s">
+        <v>41</v>
+      </c>
+      <c r="C154">
+        <v>2010</v>
+      </c>
+      <c r="D154">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>52</v>
+      </c>
+      <c r="B155" t="s">
+        <v>41</v>
+      </c>
+      <c r="C155">
+        <v>2010</v>
+      </c>
+      <c r="D155">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>53</v>
+      </c>
+      <c r="B156" t="s">
+        <v>41</v>
+      </c>
+      <c r="C156">
+        <v>2010</v>
+      </c>
+      <c r="D156">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>54</v>
+      </c>
+      <c r="B157" t="s">
+        <v>41</v>
+      </c>
+      <c r="C157">
+        <v>2010</v>
+      </c>
+      <c r="D157">
+        <v>5.8082705070489418E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>55</v>
+      </c>
+      <c r="B158" t="s">
+        <v>41</v>
+      </c>
+      <c r="C158">
+        <v>2010</v>
+      </c>
+      <c r="D158">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>56</v>
+      </c>
+      <c r="B159" t="s">
+        <v>41</v>
+      </c>
+      <c r="C159">
+        <v>2010</v>
+      </c>
+      <c r="D159">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>57</v>
+      </c>
+      <c r="B160" t="s">
+        <v>41</v>
+      </c>
+      <c r="C160">
+        <v>2010</v>
+      </c>
+      <c r="D160">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>58</v>
+      </c>
+      <c r="B161" t="s">
+        <v>41</v>
+      </c>
+      <c r="C161">
+        <v>2010</v>
+      </c>
+      <c r="D161">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>59</v>
+      </c>
+      <c r="B162" t="s">
+        <v>41</v>
+      </c>
+      <c r="C162">
+        <v>2010</v>
+      </c>
+      <c r="D162">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>60</v>
+      </c>
+      <c r="B163" t="s">
+        <v>41</v>
+      </c>
+      <c r="C163">
+        <v>2010</v>
+      </c>
+      <c r="D163">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>61</v>
+      </c>
+      <c r="B164" t="s">
+        <v>41</v>
+      </c>
+      <c r="C164">
+        <v>2010</v>
+      </c>
+      <c r="D164">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>62</v>
+      </c>
+      <c r="B165" t="s">
+        <v>41</v>
+      </c>
+      <c r="C165">
+        <v>2010</v>
+      </c>
+      <c r="D165">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>63</v>
+      </c>
+      <c r="B166" t="s">
+        <v>41</v>
+      </c>
+      <c r="C166">
+        <v>2010</v>
+      </c>
+      <c r="D166">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>64</v>
+      </c>
+      <c r="B167" t="s">
+        <v>41</v>
+      </c>
+      <c r="C167">
+        <v>2010</v>
+      </c>
+      <c r="D167">
+        <v>8.2223593877876391E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>65</v>
+      </c>
+      <c r="B168" t="s">
+        <v>41</v>
+      </c>
+      <c r="C168">
+        <v>2010</v>
+      </c>
+      <c r="D168">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>66</v>
+      </c>
+      <c r="B169" t="s">
+        <v>41</v>
+      </c>
+      <c r="C169">
+        <v>2010</v>
+      </c>
+      <c r="D169">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>67</v>
+      </c>
+      <c r="B170" t="s">
+        <v>41</v>
+      </c>
+      <c r="C170">
+        <v>2010</v>
+      </c>
+      <c r="D170">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>68</v>
+      </c>
+      <c r="B171" t="s">
+        <v>41</v>
+      </c>
+      <c r="C171">
+        <v>2010</v>
+      </c>
+      <c r="D171">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>69</v>
+      </c>
+      <c r="B172" t="s">
+        <v>41</v>
+      </c>
+      <c r="C172">
+        <v>2010</v>
+      </c>
+      <c r="D172">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>70</v>
+      </c>
+      <c r="B173" t="s">
+        <v>41</v>
+      </c>
+      <c r="C173">
+        <v>2010</v>
+      </c>
+      <c r="D173">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>71</v>
+      </c>
+      <c r="B174" t="s">
+        <v>41</v>
+      </c>
+      <c r="C174">
+        <v>2010</v>
+      </c>
+      <c r="D174">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>72</v>
+      </c>
+      <c r="B175" t="s">
+        <v>41</v>
+      </c>
+      <c r="C175">
+        <v>2010</v>
+      </c>
+      <c r="D175">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>73</v>
+      </c>
+      <c r="B176" t="s">
+        <v>41</v>
+      </c>
+      <c r="C176">
+        <v>2010</v>
+      </c>
+      <c r="D176">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>74</v>
+      </c>
+      <c r="B177" t="s">
+        <v>41</v>
+      </c>
+      <c r="C177">
+        <v>2010</v>
+      </c>
+      <c r="D177">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>75</v>
+      </c>
+      <c r="B178" t="s">
+        <v>41</v>
+      </c>
+      <c r="C178">
+        <v>2010</v>
+      </c>
+      <c r="D178">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>76</v>
+      </c>
+      <c r="B179" t="s">
+        <v>41</v>
+      </c>
+      <c r="C179">
+        <v>2010</v>
+      </c>
+      <c r="D179">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>77</v>
+      </c>
+      <c r="B180" t="s">
+        <v>41</v>
+      </c>
+      <c r="C180">
+        <v>2010</v>
+      </c>
+      <c r="D180">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>78</v>
+      </c>
+      <c r="B181" t="s">
+        <v>41</v>
+      </c>
+      <c r="C181">
+        <v>2010</v>
+      </c>
+      <c r="D181">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>79</v>
+      </c>
+      <c r="B182" t="s">
+        <v>41</v>
+      </c>
+      <c r="C182">
+        <v>2010</v>
+      </c>
+      <c r="D182">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>80</v>
+      </c>
+      <c r="B183" t="s">
+        <v>41</v>
+      </c>
+      <c r="C183">
+        <v>2010</v>
+      </c>
+      <c r="D183">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>81</v>
+      </c>
+      <c r="B184" t="s">
+        <v>41</v>
+      </c>
+      <c r="C184">
+        <v>2010</v>
+      </c>
+      <c r="D184">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>82</v>
+      </c>
+      <c r="B185" t="s">
+        <v>41</v>
+      </c>
+      <c r="C185">
+        <v>2010</v>
+      </c>
+      <c r="D185">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>83</v>
+      </c>
+      <c r="B186" t="s">
+        <v>41</v>
+      </c>
+      <c r="C186">
+        <v>2010</v>
+      </c>
+      <c r="D186">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>84</v>
+      </c>
+      <c r="B187" t="s">
+        <v>41</v>
+      </c>
+      <c r="C187">
+        <v>2010</v>
+      </c>
+      <c r="D187">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>85</v>
+      </c>
+      <c r="B188" t="s">
+        <v>41</v>
+      </c>
+      <c r="C188">
+        <v>2010</v>
+      </c>
+      <c r="D188">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>86</v>
+      </c>
+      <c r="B189" t="s">
+        <v>41</v>
+      </c>
+      <c r="C189">
+        <v>2010</v>
+      </c>
+      <c r="D189">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>87</v>
+      </c>
+      <c r="B190" t="s">
+        <v>41</v>
+      </c>
+      <c r="C190">
+        <v>2010</v>
+      </c>
+      <c r="D190">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>88</v>
+      </c>
+      <c r="B191" t="s">
+        <v>41</v>
+      </c>
+      <c r="C191">
+        <v>2010</v>
+      </c>
+      <c r="D191">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>89</v>
+      </c>
+      <c r="B192" t="s">
+        <v>41</v>
+      </c>
+      <c r="C192">
+        <v>2010</v>
+      </c>
+      <c r="D192">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>90</v>
+      </c>
+      <c r="B193" t="s">
+        <v>41</v>
+      </c>
+      <c r="C193">
+        <v>2010</v>
+      </c>
+      <c r="D193">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>91</v>
+      </c>
+      <c r="B194" t="s">
+        <v>41</v>
+      </c>
+      <c r="C194">
+        <v>2010</v>
+      </c>
+      <c r="D194">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>92</v>
+      </c>
+      <c r="B195" t="s">
+        <v>41</v>
+      </c>
+      <c r="C195">
+        <v>2010</v>
+      </c>
+      <c r="D195">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>93</v>
+      </c>
+      <c r="B196" t="s">
+        <v>41</v>
+      </c>
+      <c r="C196">
+        <v>2010</v>
+      </c>
+      <c r="D196">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>94</v>
+      </c>
+      <c r="B197" t="s">
+        <v>41</v>
+      </c>
+      <c r="C197">
+        <v>2010</v>
+      </c>
+      <c r="D197">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>95</v>
+      </c>
+      <c r="B198" t="s">
+        <v>41</v>
+      </c>
+      <c r="C198">
+        <v>2010</v>
+      </c>
+      <c r="D198">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>96</v>
+      </c>
+      <c r="B199" t="s">
+        <v>41</v>
+      </c>
+      <c r="C199">
+        <v>2010</v>
+      </c>
+      <c r="D199">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>97</v>
+      </c>
+      <c r="B200" t="s">
+        <v>41</v>
+      </c>
+      <c r="C200">
+        <v>2010</v>
+      </c>
+      <c r="D200">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>98</v>
+      </c>
+      <c r="B201" t="s">
+        <v>41</v>
+      </c>
+      <c r="C201">
+        <v>2010</v>
+      </c>
+      <c r="D201">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>99</v>
+      </c>
+      <c r="B202" t="s">
+        <v>41</v>
+      </c>
+      <c r="C202">
+        <v>2010</v>
+      </c>
+      <c r="D202">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>100</v>
+      </c>
+      <c r="B203" t="s">
+        <v>41</v>
+      </c>
+      <c r="C203">
+        <v>2010</v>
+      </c>
+      <c r="D203">
+        <v>1.1631675388387665E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3435"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2044" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3248" sqref="F3248:F3249"/>
     </sheetView>
   </sheetViews>
@@ -69746,7 +72616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -69812,7 +72682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D163"/>
   <sheetViews>
@@ -72109,7 +74979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -72525,10 +75395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -72590,7 +75460,7 @@
         <v>166</v>
       </c>
       <c r="B7" s="28">
-        <v>0.68</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -72598,39 +75468,39 @@
         <v>167</v>
       </c>
       <c r="B8" s="28">
-        <v>0.22</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B9" s="28">
-        <v>0.73</v>
+        <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B10" s="28">
-        <v>2.7000000000000001E-3</v>
+        <v>1.1599999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B11" s="28">
-        <v>1.1599999999999999E-2</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>143</v>
+        <v>207</v>
       </c>
       <c r="B12" s="28">
-        <v>1E-4</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -72643,7 +75513,7 @@
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="28">
         <v>0.05</v>
@@ -72651,7 +75521,7 @@
     </row>
     <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="28">
         <v>0.5</v>
@@ -72659,7 +75529,7 @@
     </row>
     <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="28">
         <v>0.25</v>
@@ -72667,7 +75537,7 @@
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17" s="28">
         <v>0.05</v>
@@ -72675,7 +75545,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18" s="28">
         <v>0.02</v>
@@ -72683,7 +75553,7 @@
     </row>
     <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" s="28">
         <v>0.15</v>
@@ -72699,297 +75569,305 @@
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="B21" s="28">
-        <v>0.8</v>
+        <v>8.2500000000000004E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B22" s="28">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B23" s="28">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24" s="28">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B25" s="28">
-        <v>0.91</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B26" s="28">
-        <v>0.89</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B27" s="28">
-        <v>0.99</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="B28" s="28">
-        <v>0.85</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="28">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B30" s="28">
-        <v>1.24E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" s="28">
-        <v>6.7699999999999996E-2</v>
+        <v>1.24E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="B32" s="28">
+        <v>6.7699999999999996E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="28">
         <v>0.35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="B33" s="25">
-        <v>0.42</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B34" s="25">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="25">
         <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="25">
-        <v>0.35</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B36" s="25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" s="25">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="B37" s="29">
-        <v>0.62</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B38" s="29">
-        <v>0.4</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="28">
-        <v>3</v>
+        <v>185</v>
+      </c>
+      <c r="B39" s="29">
+        <v>0.4</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" s="28">
-        <v>2.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="28">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="28">
+      <c r="B42" s="28">
         <v>2.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B42" s="25">
-        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B43" s="25">
-        <v>548</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B44" s="25">
-        <v>0.4</v>
+        <v>548</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B45" s="25">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B46" s="25">
-        <v>0.68</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B47" s="25">
-        <v>0.86</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B48" s="25">
-        <v>0.76</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B49" s="25">
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" s="25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" s="25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B50" s="25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B51" s="25">
+      <c r="B52" s="25">
         <v>0.82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="B52" s="25">
-        <v>0.81</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B53" s="25">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B54" s="25">
-        <v>0.61</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B55" s="25">
-        <v>0.78500000000000003</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B56" s="25">
-        <v>0.78200000000000003</v>
+        <v>0.78500000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B57" s="25">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="25">
         <v>0.84399999999999997</v>
       </c>
     </row>
@@ -75426,23 +78304,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>156</v>
       </c>
@@ -75450,19 +78330,25 @@
         <v>157</v>
       </c>
       <c r="C1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" t="s">
         <v>158</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -75473,16 +78359,22 @@
         <v>2</v>
       </c>
       <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -75493,16 +78385,22 @@
         <v>4</v>
       </c>
       <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -75513,151 +78411,205 @@
         <v>8</v>
       </c>
       <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>8</v>
       </c>
-      <c r="F4">
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
       <c r="C6">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>24</v>
       </c>
-      <c r="E8">
+      <c r="D8">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>28</v>
       </c>
-      <c r="E9">
+      <c r="D9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10">
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11">
+      <c r="F10">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12">
+      <c r="F11">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14">
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27">
         <v>100</v>
       </c>
     </row>
@@ -76183,7 +79135,7 @@
   <dimension ref="A1:D203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tb mortality rates high and tb transmission rate high
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -75398,7 +75398,7 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75452,7 +75452,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="25">
-        <v>0.75</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -77965,7 +77965,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add risk of progression to active tb for aids patients
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7745" uniqueCount="210">
   <si>
     <t>Name:</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>monthly_prob_self_cure_hiv</t>
+  </si>
+  <si>
+    <t>rr_tb_aids</t>
   </si>
 </sst>
 </file>
@@ -75395,10 +75398,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75688,186 +75691,194 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
-        <v>182</v>
+      <c r="A36" s="24" t="s">
+        <v>209</v>
       </c>
       <c r="B36" s="25">
-        <v>0.35</v>
+        <v>26.06</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B38" s="25">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="B38" s="29">
-        <v>0.62</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B39" s="29">
-        <v>0.4</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="28">
-        <v>3</v>
+        <v>185</v>
+      </c>
+      <c r="B40" s="29">
+        <v>0.4</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B41" s="28">
-        <v>2.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="28">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B43" s="28">
         <v>2.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="B43" s="25">
-        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B44" s="25">
-        <v>548</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B45" s="25">
-        <v>0.4</v>
+        <v>548</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B46" s="25">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B47" s="25">
-        <v>0.68</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B48" s="25">
-        <v>0.86</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B49" s="25">
-        <v>0.76</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B50" s="25">
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B51" s="25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="B51" s="25">
+      <c r="B52" s="25">
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B53" s="25">
         <v>0.82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="B53" s="25">
-        <v>0.81</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B54" s="25">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B55" s="25">
-        <v>0.61</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B56" s="25">
-        <v>0.78500000000000003</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B57" s="25">
-        <v>0.78200000000000003</v>
+        <v>0.78500000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58" s="25">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="B58" s="25">
+      <c r="B59" s="25">
         <v>0.84399999999999997</v>
       </c>
     </row>
@@ -77965,7 +77976,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD16"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
link to aids onset once hiv+ person gets active tb
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -75400,8 +75400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75455,7 +75455,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="25">
-        <v>0.03</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
calibration runs with additional logging
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" activeTab="3"/>
+    <workbookView xWindow="12210" yWindow="15" windowWidth="10740" windowHeight="11835" tabRatio="731" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7745" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7947" uniqueCount="212">
   <si>
     <t>Name:</t>
   </si>
@@ -682,6 +682,12 @@
   <si>
     <t>rr_tb_aids</t>
   </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
 </sst>
 </file>
 
@@ -951,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1026,6 +1032,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -75041,12 +75048,12 @@
   <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -75400,7 +75407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -75890,19 +75897,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" style="30"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="30" t="s">
         <v>154</v>
       </c>
       <c r="C1" t="s">
@@ -75913,8 +75923,8 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
+      <c r="B2" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C2">
         <v>0.7</v>
@@ -75924,8 +75934,8 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
+      <c r="B3" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C3">
         <v>0.74</v>
@@ -75935,8 +75945,8 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="b">
-        <v>0</v>
+      <c r="B4" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C4">
         <v>0.91</v>
@@ -75946,8 +75956,8 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
+      <c r="B5" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C5">
         <v>0.91</v>
@@ -75957,8 +75967,8 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
+      <c r="B6" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C6">
         <v>0.91</v>
@@ -75968,8 +75978,8 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="b">
-        <v>0</v>
+      <c r="B7" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C7">
         <v>0.89</v>
@@ -75979,8 +75989,8 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
+      <c r="B8" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C8">
         <v>0.89</v>
@@ -75990,8 +76000,8 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="b">
-        <v>0</v>
+      <c r="B9" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C9">
         <v>0.89</v>
@@ -76001,8 +76011,8 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="b">
-        <v>0</v>
+      <c r="B10" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C10">
         <v>0.89</v>
@@ -76012,8 +76022,8 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
+      <c r="B11" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C11">
         <v>0.89</v>
@@ -76023,8 +76033,8 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="b">
-        <v>0</v>
+      <c r="B12" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C12">
         <v>0.99</v>
@@ -76034,8 +76044,8 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
+      <c r="B13" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C13">
         <v>0.99</v>
@@ -76045,8 +76055,8 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="b">
-        <v>0</v>
+      <c r="B14" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C14">
         <v>0.99</v>
@@ -76056,8 +76066,8 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
+      <c r="B15" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C15">
         <v>0.99</v>
@@ -76067,8 +76077,8 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
+      <c r="B16" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C16">
         <v>0.99</v>
@@ -76078,8 +76088,8 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
+      <c r="B17" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C17">
         <v>0.8</v>
@@ -76089,8 +76099,8 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
+      <c r="B18" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C18">
         <v>0.8</v>
@@ -76100,8 +76110,8 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="b">
-        <v>0</v>
+      <c r="B19" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C19">
         <v>0.8</v>
@@ -76111,8 +76121,8 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="b">
-        <v>0</v>
+      <c r="B20" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C20">
         <v>0.8</v>
@@ -76122,8 +76132,8 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="b">
-        <v>0</v>
+      <c r="B21" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C21">
         <v>0.8</v>
@@ -76133,8 +76143,8 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="b">
-        <v>0</v>
+      <c r="B22" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C22">
         <v>0.8</v>
@@ -76144,8 +76154,8 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="b">
-        <v>0</v>
+      <c r="B23" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C23">
         <v>0.8</v>
@@ -76155,8 +76165,8 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="b">
-        <v>0</v>
+      <c r="B24" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C24">
         <v>0.8</v>
@@ -76166,8 +76176,8 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="b">
-        <v>0</v>
+      <c r="B25" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C25">
         <v>0.8</v>
@@ -76177,8 +76187,8 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="b">
-        <v>0</v>
+      <c r="B26" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C26">
         <v>0.8</v>
@@ -76188,8 +76198,8 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="b">
-        <v>0</v>
+      <c r="B27" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C27">
         <v>0.8</v>
@@ -76199,8 +76209,8 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="b">
-        <v>0</v>
+      <c r="B28" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C28">
         <v>0.8</v>
@@ -76210,8 +76220,8 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="b">
-        <v>0</v>
+      <c r="B29" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C29">
         <v>0.8</v>
@@ -76221,8 +76231,8 @@
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="b">
-        <v>0</v>
+      <c r="B30" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C30">
         <v>0.8</v>
@@ -76232,8 +76242,8 @@
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="b">
-        <v>0</v>
+      <c r="B31" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C31">
         <v>0.8</v>
@@ -76243,8 +76253,8 @@
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="b">
-        <v>0</v>
+      <c r="B32" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C32">
         <v>0.8</v>
@@ -76254,8 +76264,8 @@
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="b">
-        <v>0</v>
+      <c r="B33" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C33">
         <v>0.8</v>
@@ -76265,8 +76275,8 @@
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="b">
-        <v>0</v>
+      <c r="B34" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C34">
         <v>0.8</v>
@@ -76276,8 +76286,8 @@
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="b">
-        <v>0</v>
+      <c r="B35" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C35">
         <v>0.8</v>
@@ -76287,8 +76297,8 @@
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="b">
-        <v>0</v>
+      <c r="B36" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C36">
         <v>0.8</v>
@@ -76298,8 +76308,8 @@
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="b">
-        <v>0</v>
+      <c r="B37" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C37">
         <v>0.8</v>
@@ -76309,8 +76319,8 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="b">
-        <v>0</v>
+      <c r="B38" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C38">
         <v>0.8</v>
@@ -76320,8 +76330,8 @@
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
+      <c r="B39" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C39">
         <v>0.8</v>
@@ -76331,8 +76341,8 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="b">
-        <v>0</v>
+      <c r="B40" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C40">
         <v>0.8</v>
@@ -76342,8 +76352,8 @@
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="b">
-        <v>0</v>
+      <c r="B41" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C41">
         <v>0.8</v>
@@ -76353,8 +76363,8 @@
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="b">
-        <v>0</v>
+      <c r="B42" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C42">
         <v>0.8</v>
@@ -76364,8 +76374,8 @@
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="b">
-        <v>0</v>
+      <c r="B43" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C43">
         <v>0.8</v>
@@ -76375,8 +76385,8 @@
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="b">
-        <v>0</v>
+      <c r="B44" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C44">
         <v>0.8</v>
@@ -76386,8 +76396,8 @@
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" t="b">
-        <v>0</v>
+      <c r="B45" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C45">
         <v>0.8</v>
@@ -76397,8 +76407,8 @@
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="b">
-        <v>0</v>
+      <c r="B46" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C46">
         <v>0.8</v>
@@ -76408,8 +76418,8 @@
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="b">
-        <v>0</v>
+      <c r="B47" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C47">
         <v>0.8</v>
@@ -76419,8 +76429,8 @@
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="b">
-        <v>0</v>
+      <c r="B48" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C48">
         <v>0.8</v>
@@ -76430,8 +76440,8 @@
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="b">
-        <v>0</v>
+      <c r="B49" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C49">
         <v>0.8</v>
@@ -76441,8 +76451,8 @@
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="b">
-        <v>0</v>
+      <c r="B50" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C50">
         <v>0.8</v>
@@ -76452,8 +76462,8 @@
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="b">
-        <v>0</v>
+      <c r="B51" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C51">
         <v>0.8</v>
@@ -76463,8 +76473,8 @@
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="b">
-        <v>0</v>
+      <c r="B52" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C52">
         <v>0.8</v>
@@ -76474,8 +76484,8 @@
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="b">
-        <v>0</v>
+      <c r="B53" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C53">
         <v>0.8</v>
@@ -76485,8 +76495,8 @@
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" t="b">
-        <v>0</v>
+      <c r="B54" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C54">
         <v>0.8</v>
@@ -76496,8 +76506,8 @@
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="b">
-        <v>0</v>
+      <c r="B55" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C55">
         <v>0.8</v>
@@ -76507,8 +76517,8 @@
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" t="b">
-        <v>0</v>
+      <c r="B56" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C56">
         <v>0.8</v>
@@ -76518,8 +76528,8 @@
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="b">
-        <v>0</v>
+      <c r="B57" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C57">
         <v>0.8</v>
@@ -76529,8 +76539,8 @@
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="b">
-        <v>0</v>
+      <c r="B58" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C58">
         <v>0.8</v>
@@ -76540,8 +76550,8 @@
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="b">
-        <v>0</v>
+      <c r="B59" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C59">
         <v>0.8</v>
@@ -76551,8 +76561,8 @@
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="b">
-        <v>0</v>
+      <c r="B60" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C60">
         <v>0.8</v>
@@ -76562,8 +76572,8 @@
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="b">
-        <v>0</v>
+      <c r="B61" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C61">
         <v>0.8</v>
@@ -76573,8 +76583,8 @@
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="b">
-        <v>0</v>
+      <c r="B62" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C62">
         <v>0.8</v>
@@ -76584,8 +76594,8 @@
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="b">
-        <v>0</v>
+      <c r="B63" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C63">
         <v>0.8</v>
@@ -76595,8 +76605,8 @@
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="b">
-        <v>0</v>
+      <c r="B64" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C64">
         <v>0.8</v>
@@ -76606,8 +76616,8 @@
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="b">
-        <v>0</v>
+      <c r="B65" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C65">
         <v>0.8</v>
@@ -76617,8 +76627,8 @@
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="b">
-        <v>0</v>
+      <c r="B66" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C66">
         <v>0.8</v>
@@ -76628,8 +76638,8 @@
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="b">
-        <v>0</v>
+      <c r="B67" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C67">
         <v>0.8</v>
@@ -76639,8 +76649,8 @@
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="b">
-        <v>0</v>
+      <c r="B68" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C68">
         <v>0.8</v>
@@ -76650,8 +76660,8 @@
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="b">
-        <v>0</v>
+      <c r="B69" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C69">
         <v>0.8</v>
@@ -76661,8 +76671,8 @@
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="b">
-        <v>0</v>
+      <c r="B70" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C70">
         <v>0.8</v>
@@ -76672,8 +76682,8 @@
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="b">
-        <v>0</v>
+      <c r="B71" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C71">
         <v>0.8</v>
@@ -76683,8 +76693,8 @@
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="b">
-        <v>0</v>
+      <c r="B72" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C72">
         <v>0.8</v>
@@ -76694,8 +76704,8 @@
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="b">
-        <v>0</v>
+      <c r="B73" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C73">
         <v>0.8</v>
@@ -76705,8 +76715,8 @@
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="b">
-        <v>0</v>
+      <c r="B74" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C74">
         <v>0.8</v>
@@ -76716,8 +76726,8 @@
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" t="b">
-        <v>0</v>
+      <c r="B75" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C75">
         <v>0.8</v>
@@ -76727,8 +76737,8 @@
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" t="b">
-        <v>0</v>
+      <c r="B76" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C76">
         <v>0.8</v>
@@ -76738,8 +76748,8 @@
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="b">
-        <v>0</v>
+      <c r="B77" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C77">
         <v>0.8</v>
@@ -76749,8 +76759,8 @@
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" t="b">
-        <v>0</v>
+      <c r="B78" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C78">
         <v>0.8</v>
@@ -76760,8 +76770,8 @@
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" t="b">
-        <v>0</v>
+      <c r="B79" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C79">
         <v>0.8</v>
@@ -76771,8 +76781,8 @@
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="b">
-        <v>0</v>
+      <c r="B80" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C80">
         <v>0.8</v>
@@ -76782,8 +76792,8 @@
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" t="b">
-        <v>0</v>
+      <c r="B81" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C81">
         <v>0.8</v>
@@ -76793,8 +76803,8 @@
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" t="b">
-        <v>0</v>
+      <c r="B82" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C82">
         <v>0.8</v>
@@ -76804,8 +76814,8 @@
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" t="b">
-        <v>0</v>
+      <c r="B83" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C83">
         <v>0.8</v>
@@ -76815,8 +76825,8 @@
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" t="b">
-        <v>0</v>
+      <c r="B84" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C84">
         <v>0.8</v>
@@ -76826,8 +76836,8 @@
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" t="b">
-        <v>0</v>
+      <c r="B85" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C85">
         <v>0.8</v>
@@ -76837,8 +76847,8 @@
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" t="b">
-        <v>0</v>
+      <c r="B86" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C86">
         <v>0.8</v>
@@ -76848,8 +76858,8 @@
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="b">
-        <v>0</v>
+      <c r="B87" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C87">
         <v>0.8</v>
@@ -76859,8 +76869,8 @@
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" t="b">
-        <v>0</v>
+      <c r="B88" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C88">
         <v>0.8</v>
@@ -76870,8 +76880,8 @@
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" t="b">
-        <v>0</v>
+      <c r="B89" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C89">
         <v>0.8</v>
@@ -76881,8 +76891,8 @@
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" t="b">
-        <v>0</v>
+      <c r="B90" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C90">
         <v>0.8</v>
@@ -76892,8 +76902,8 @@
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" t="b">
-        <v>0</v>
+      <c r="B91" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C91">
         <v>0.8</v>
@@ -76903,8 +76913,8 @@
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" t="b">
-        <v>0</v>
+      <c r="B92" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C92">
         <v>0.8</v>
@@ -76914,8 +76924,8 @@
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" t="b">
-        <v>0</v>
+      <c r="B93" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C93">
         <v>0.8</v>
@@ -76925,8 +76935,8 @@
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" t="b">
-        <v>0</v>
+      <c r="B94" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C94">
         <v>0.8</v>
@@ -76936,8 +76946,8 @@
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" t="b">
-        <v>0</v>
+      <c r="B95" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C95">
         <v>0.8</v>
@@ -76947,8 +76957,8 @@
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" t="b">
-        <v>0</v>
+      <c r="B96" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C96">
         <v>0.8</v>
@@ -76958,8 +76968,8 @@
       <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" t="b">
-        <v>0</v>
+      <c r="B97" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C97">
         <v>0.8</v>
@@ -76969,8 +76979,8 @@
       <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" t="b">
-        <v>0</v>
+      <c r="B98" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C98">
         <v>0.8</v>
@@ -76980,8 +76990,8 @@
       <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" t="b">
-        <v>0</v>
+      <c r="B99" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C99">
         <v>0.8</v>
@@ -76991,8 +77001,8 @@
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" t="b">
-        <v>0</v>
+      <c r="B100" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C100">
         <v>0.8</v>
@@ -77002,8 +77012,8 @@
       <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" t="b">
-        <v>0</v>
+      <c r="B101" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C101">
         <v>0.8</v>
@@ -77013,8 +77023,8 @@
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" t="b">
-        <v>0</v>
+      <c r="B102" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="C102">
         <v>0.8</v>
@@ -77022,10 +77032,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>15</v>
-      </c>
-      <c r="B103" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C103">
         <v>0.5</v>
@@ -77033,10 +77043,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>16</v>
-      </c>
-      <c r="B104" t="b">
         <v>1</v>
+      </c>
+      <c r="B104" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C104">
         <v>0.5</v>
@@ -77044,10 +77054,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>17</v>
-      </c>
-      <c r="B105" t="b">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B105" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C105">
         <v>0.5</v>
@@ -77055,10 +77065,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>18</v>
-      </c>
-      <c r="B106" t="b">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B106" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C106">
         <v>0.5</v>
@@ -77066,10 +77076,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>19</v>
-      </c>
-      <c r="B107" t="b">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B107" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C107">
         <v>0.5</v>
@@ -77077,10 +77087,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>20</v>
-      </c>
-      <c r="B108" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C108">
         <v>0.5</v>
@@ -77088,10 +77098,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>21</v>
-      </c>
-      <c r="B109" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B109" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C109">
         <v>0.5</v>
@@ -77099,10 +77109,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>22</v>
-      </c>
-      <c r="B110" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C110">
         <v>0.5</v>
@@ -77110,10 +77120,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>23</v>
-      </c>
-      <c r="B111" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C111">
         <v>0.5</v>
@@ -77121,10 +77131,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>24</v>
-      </c>
-      <c r="B112" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B112" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C112">
         <v>0.5</v>
@@ -77132,10 +77142,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>25</v>
-      </c>
-      <c r="B113" t="b">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B113" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C113">
         <v>0.5</v>
@@ -77143,10 +77153,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>26</v>
-      </c>
-      <c r="B114" t="b">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B114" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C114">
         <v>0.5</v>
@@ -77154,10 +77164,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>27</v>
-      </c>
-      <c r="B115" t="b">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B115" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C115">
         <v>0.5</v>
@@ -77165,10 +77175,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>28</v>
-      </c>
-      <c r="B116" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C116">
         <v>0.5</v>
@@ -77176,10 +77186,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>29</v>
-      </c>
-      <c r="B117" t="b">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B117" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C117">
         <v>0.5</v>
@@ -77187,10 +77197,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>30</v>
-      </c>
-      <c r="B118" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B118" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C118">
         <v>0.5</v>
@@ -77198,10 +77208,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>31</v>
-      </c>
-      <c r="B119" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B119" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C119">
         <v>0.5</v>
@@ -77209,10 +77219,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>32</v>
-      </c>
-      <c r="B120" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B120" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C120">
         <v>0.5</v>
@@ -77220,10 +77230,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>33</v>
-      </c>
-      <c r="B121" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C121">
         <v>0.5</v>
@@ -77231,10 +77241,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>34</v>
-      </c>
-      <c r="B122" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B122" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C122">
         <v>0.5</v>
@@ -77242,10 +77252,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>35</v>
-      </c>
-      <c r="B123" t="b">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C123">
         <v>0.5</v>
@@ -77253,10 +77263,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>36</v>
-      </c>
-      <c r="B124" t="b">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C124">
         <v>0.5</v>
@@ -77264,10 +77274,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>37</v>
-      </c>
-      <c r="B125" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B125" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C125">
         <v>0.5</v>
@@ -77275,10 +77285,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>38</v>
-      </c>
-      <c r="B126" t="b">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B126" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C126">
         <v>0.5</v>
@@ -77286,10 +77296,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>39</v>
-      </c>
-      <c r="B127" t="b">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="B127" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C127">
         <v>0.5</v>
@@ -77297,10 +77307,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>40</v>
-      </c>
-      <c r="B128" t="b">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B128" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C128">
         <v>0.5</v>
@@ -77308,10 +77318,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>41</v>
-      </c>
-      <c r="B129" t="b">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B129" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C129">
         <v>0.5</v>
@@ -77319,10 +77329,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>42</v>
-      </c>
-      <c r="B130" t="b">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="B130" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C130">
         <v>0.5</v>
@@ -77330,10 +77340,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>43</v>
-      </c>
-      <c r="B131" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="B131" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C131">
         <v>0.5</v>
@@ -77341,10 +77351,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>44</v>
-      </c>
-      <c r="B132" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B132" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C132">
         <v>0.5</v>
@@ -77352,10 +77362,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>45</v>
-      </c>
-      <c r="B133" t="b">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B133" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C133">
         <v>0.5</v>
@@ -77363,10 +77373,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>46</v>
-      </c>
-      <c r="B134" t="b">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B134" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C134">
         <v>0.5</v>
@@ -77374,10 +77384,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>47</v>
-      </c>
-      <c r="B135" t="b">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="B135" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C135">
         <v>0.5</v>
@@ -77385,10 +77395,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>48</v>
-      </c>
-      <c r="B136" t="b">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C136">
         <v>0.5</v>
@@ -77396,10 +77406,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>49</v>
-      </c>
-      <c r="B137" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="B137" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C137">
         <v>0.5</v>
@@ -77407,10 +77417,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>50</v>
-      </c>
-      <c r="B138" t="b">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B138" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C138">
         <v>0.5</v>
@@ -77418,10 +77428,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>51</v>
-      </c>
-      <c r="B139" t="b">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="B139" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C139">
         <v>0.5</v>
@@ -77429,10 +77439,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>52</v>
-      </c>
-      <c r="B140" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="B140" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C140">
         <v>0.5</v>
@@ -77440,10 +77450,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>53</v>
-      </c>
-      <c r="B141" t="b">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="B141" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C141">
         <v>0.5</v>
@@ -77451,10 +77461,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>54</v>
-      </c>
-      <c r="B142" t="b">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B142" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C142">
         <v>0.5</v>
@@ -77462,10 +77472,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>55</v>
-      </c>
-      <c r="B143" t="b">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B143" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C143">
         <v>0.5</v>
@@ -77473,10 +77483,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>56</v>
-      </c>
-      <c r="B144" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B144" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C144">
         <v>0.5</v>
@@ -77484,10 +77494,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>57</v>
-      </c>
-      <c r="B145" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="B145" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C145">
         <v>0.5</v>
@@ -77495,10 +77505,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>58</v>
-      </c>
-      <c r="B146" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="B146" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C146">
         <v>0.5</v>
@@ -77506,10 +77516,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>59</v>
-      </c>
-      <c r="B147" t="b">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B147" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C147">
         <v>0.5</v>
@@ -77517,10 +77527,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>60</v>
-      </c>
-      <c r="B148" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="B148" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C148">
         <v>0.5</v>
@@ -77528,10 +77538,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>61</v>
-      </c>
-      <c r="B149" t="b">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B149" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C149">
         <v>0.5</v>
@@ -77539,10 +77549,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>62</v>
-      </c>
-      <c r="B150" t="b">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="B150" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C150">
         <v>0.5</v>
@@ -77550,10 +77560,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>63</v>
-      </c>
-      <c r="B151" t="b">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="B151" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C151">
         <v>0.5</v>
@@ -77561,10 +77571,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>64</v>
-      </c>
-      <c r="B152" t="b">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="B152" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C152">
         <v>0.5</v>
@@ -77572,10 +77582,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>65</v>
-      </c>
-      <c r="B153" t="b">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="B153" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C153">
         <v>0.5</v>
@@ -77583,10 +77593,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>66</v>
-      </c>
-      <c r="B154" t="b">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="B154" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C154">
         <v>0.5</v>
@@ -77594,10 +77604,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>67</v>
-      </c>
-      <c r="B155" t="b">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="B155" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C155">
         <v>0.5</v>
@@ -77605,10 +77615,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>68</v>
-      </c>
-      <c r="B156" t="b">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="B156" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C156">
         <v>0.5</v>
@@ -77616,10 +77626,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>69</v>
-      </c>
-      <c r="B157" t="b">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="B157" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C157">
         <v>0.5</v>
@@ -77627,10 +77637,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>70</v>
-      </c>
-      <c r="B158" t="b">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B158" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C158">
         <v>0.5</v>
@@ -77638,10 +77648,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>71</v>
-      </c>
-      <c r="B159" t="b">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="B159" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C159">
         <v>0.5</v>
@@ -77649,10 +77659,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>72</v>
-      </c>
-      <c r="B160" t="b">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="B160" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C160">
         <v>0.5</v>
@@ -77660,10 +77670,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>73</v>
-      </c>
-      <c r="B161" t="b">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="B161" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C161">
         <v>0.5</v>
@@ -77671,10 +77681,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>74</v>
-      </c>
-      <c r="B162" t="b">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B162" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C162">
         <v>0.5</v>
@@ -77682,10 +77692,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>75</v>
-      </c>
-      <c r="B163" t="b">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="B163" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C163">
         <v>0.5</v>
@@ -77693,10 +77703,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>76</v>
-      </c>
-      <c r="B164" t="b">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B164" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C164">
         <v>0.5</v>
@@ -77704,10 +77714,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>77</v>
-      </c>
-      <c r="B165" t="b">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B165" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C165">
         <v>0.5</v>
@@ -77715,10 +77725,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>78</v>
-      </c>
-      <c r="B166" t="b">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B166" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C166">
         <v>0.5</v>
@@ -77726,10 +77736,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>79</v>
-      </c>
-      <c r="B167" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="B167" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C167">
         <v>0.5</v>
@@ -77737,10 +77747,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>80</v>
-      </c>
-      <c r="B168" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B168" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C168">
         <v>0.5</v>
@@ -77748,10 +77758,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>81</v>
-      </c>
-      <c r="B169" t="b">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="B169" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C169">
         <v>0.5</v>
@@ -77759,10 +77769,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>82</v>
-      </c>
-      <c r="B170" t="b">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B170" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C170">
         <v>0.5</v>
@@ -77770,10 +77780,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>83</v>
-      </c>
-      <c r="B171" t="b">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B171" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C171">
         <v>0.5</v>
@@ -77781,10 +77791,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>84</v>
-      </c>
-      <c r="B172" t="b">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="B172" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C172">
         <v>0.5</v>
@@ -77792,10 +77802,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>85</v>
-      </c>
-      <c r="B173" t="b">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B173" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C173">
         <v>0.5</v>
@@ -77803,10 +77813,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>86</v>
-      </c>
-      <c r="B174" t="b">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="B174" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C174">
         <v>0.5</v>
@@ -77814,10 +77824,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>87</v>
-      </c>
-      <c r="B175" t="b">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B175" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C175">
         <v>0.5</v>
@@ -77825,10 +77835,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>88</v>
-      </c>
-      <c r="B176" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="B176" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C176">
         <v>0.5</v>
@@ -77836,10 +77846,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>89</v>
-      </c>
-      <c r="B177" t="b">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B177" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C177">
         <v>0.5</v>
@@ -77847,10 +77857,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>90</v>
-      </c>
-      <c r="B178" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="B178" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C178">
         <v>0.5</v>
@@ -77858,10 +77868,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>91</v>
-      </c>
-      <c r="B179" t="b">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="B179" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C179">
         <v>0.5</v>
@@ -77869,10 +77879,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>92</v>
-      </c>
-      <c r="B180" t="b">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="B180" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C180">
         <v>0.5</v>
@@ -77880,10 +77890,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>93</v>
-      </c>
-      <c r="B181" t="b">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B181" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C181">
         <v>0.5</v>
@@ -77891,10 +77901,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>94</v>
-      </c>
-      <c r="B182" t="b">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="B182" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C182">
         <v>0.5</v>
@@ -77902,10 +77912,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>95</v>
-      </c>
-      <c r="B183" t="b">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="B183" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C183">
         <v>0.5</v>
@@ -77913,10 +77923,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>96</v>
-      </c>
-      <c r="B184" t="b">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="B184" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C184">
         <v>0.5</v>
@@ -77924,10 +77934,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>97</v>
-      </c>
-      <c r="B185" t="b">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="B185" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C185">
         <v>0.5</v>
@@ -77935,10 +77945,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>98</v>
-      </c>
-      <c r="B186" t="b">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="B186" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C186">
         <v>0.5</v>
@@ -77946,10 +77956,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>99</v>
-      </c>
-      <c r="B187" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="B187" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="C187">
         <v>0.5</v>
@@ -77957,12 +77967,177 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
+        <v>85</v>
+      </c>
+      <c r="B188" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C188">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>86</v>
+      </c>
+      <c r="B189" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C189">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>87</v>
+      </c>
+      <c r="B190" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C190">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>88</v>
+      </c>
+      <c r="B191" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C191">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>89</v>
+      </c>
+      <c r="B192" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C192">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>90</v>
+      </c>
+      <c r="B193" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C193">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>91</v>
+      </c>
+      <c r="B194" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C194">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>92</v>
+      </c>
+      <c r="B195" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C195">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>93</v>
+      </c>
+      <c r="B196" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C196">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>94</v>
+      </c>
+      <c r="B197" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C197">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>95</v>
+      </c>
+      <c r="B198" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C198">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>96</v>
+      </c>
+      <c r="B199" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C199">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>97</v>
+      </c>
+      <c r="B200" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C200">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>98</v>
+      </c>
+      <c r="B201" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C201">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>99</v>
+      </c>
+      <c r="B202" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C202">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
         <v>100</v>
       </c>
-      <c r="B188" t="b">
-        <v>1</v>
-      </c>
-      <c r="C188">
+      <c r="B203" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C203">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edits to tb active progression for calibration
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -1087,12 +1087,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1102,6 +1096,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -77972,12 +77972,12 @@
   <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -78331,8 +78331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -78442,7 +78442,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="28">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -78490,7 +78490,7 @@
         <v>171</v>
       </c>
       <c r="B19" s="28">
-        <v>0.15</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -78814,10 +78814,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="36">
+      <c r="B60" s="34">
         <v>0.75</v>
       </c>
     </row>
@@ -78837,61 +78837,61 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="33"/>
+    <col min="1" max="1" width="9" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="31" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="31" t="s">
         <v>222</v>
       </c>
     </row>
@@ -81157,7 +81157,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove health system constraints for faster run time
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -78331,7 +78331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -78386,7 +78386,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="25">
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
bcg coverage in infants close to data estimates
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,8 @@
     <sheet name="latent_TB2014_summary" sheetId="11" r:id="rId13"/>
     <sheet name="Latent_TB_prob" sheetId="13" r:id="rId14"/>
     <sheet name="WHO_estimates" sheetId="24" r:id="rId15"/>
-    <sheet name="BCG" sheetId="25" r:id="rId16"/>
-    <sheet name="BCG_baseline" sheetId="26" r:id="rId17"/>
+    <sheet name="BCG_baseline" sheetId="26" r:id="rId16"/>
+    <sheet name="BCG" sheetId="25" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Active_TB_prob!$A$1:$F$3435</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8113" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8113" uniqueCount="334">
   <si>
     <t>Name:</t>
   </si>
@@ -744,9 +744,6 @@
   </si>
   <si>
     <t>prevalence_all_ages_high</t>
-  </si>
-  <si>
-    <t>Malawi</t>
   </si>
   <si>
     <t>BCG immunization coverage among 1-year-olds (%)</t>
@@ -78252,7 +78249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -78282,7 +78279,7 @@
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -79298,461 +79295,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2">
-        <v>2018</v>
-      </c>
-      <c r="C2">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3">
-        <v>2017</v>
-      </c>
-      <c r="C3">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4">
-        <v>2016</v>
-      </c>
-      <c r="C4">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5">
-        <v>2015</v>
-      </c>
-      <c r="C5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B6">
-        <v>2014</v>
-      </c>
-      <c r="C6">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7">
-        <v>2013</v>
-      </c>
-      <c r="C7">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B8">
-        <v>2012</v>
-      </c>
-      <c r="C8">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B9">
-        <v>2011</v>
-      </c>
-      <c r="C9">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10">
-        <v>2010</v>
-      </c>
-      <c r="C10">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11">
-        <v>2009</v>
-      </c>
-      <c r="C11">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>231</v>
-      </c>
-      <c r="B12">
-        <v>2008</v>
-      </c>
-      <c r="C12">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B13">
-        <v>2007</v>
-      </c>
-      <c r="C13">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>231</v>
-      </c>
-      <c r="B14">
-        <v>2006</v>
-      </c>
-      <c r="C14">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15">
-        <v>2005</v>
-      </c>
-      <c r="C15">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>231</v>
-      </c>
-      <c r="B16">
-        <v>2004</v>
-      </c>
-      <c r="C16">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B17">
-        <v>2003</v>
-      </c>
-      <c r="C17">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>231</v>
-      </c>
-      <c r="B18">
-        <v>2002</v>
-      </c>
-      <c r="C18">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>231</v>
-      </c>
-      <c r="B19">
-        <v>2001</v>
-      </c>
-      <c r="C19">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B20">
-        <v>2000</v>
-      </c>
-      <c r="C20">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>231</v>
-      </c>
-      <c r="B21">
-        <v>1999</v>
-      </c>
-      <c r="C21">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>231</v>
-      </c>
-      <c r="B22">
-        <v>1998</v>
-      </c>
-      <c r="C22">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>231</v>
-      </c>
-      <c r="B23">
-        <v>1997</v>
-      </c>
-      <c r="C23">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>231</v>
-      </c>
-      <c r="B24">
-        <v>1996</v>
-      </c>
-      <c r="C24">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>231</v>
-      </c>
-      <c r="B25">
-        <v>1995</v>
-      </c>
-      <c r="C25">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>231</v>
-      </c>
-      <c r="B26">
-        <v>1994</v>
-      </c>
-      <c r="C26">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>231</v>
-      </c>
-      <c r="B27">
-        <v>1993</v>
-      </c>
-      <c r="C27">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B28">
-        <v>1992</v>
-      </c>
-      <c r="C28">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>231</v>
-      </c>
-      <c r="B29">
-        <v>1991</v>
-      </c>
-      <c r="C29">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>231</v>
-      </c>
-      <c r="B30">
-        <v>1990</v>
-      </c>
-      <c r="C30">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>231</v>
-      </c>
-      <c r="B31">
-        <v>1989</v>
-      </c>
-      <c r="C31">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>231</v>
-      </c>
-      <c r="B32">
-        <v>1988</v>
-      </c>
-      <c r="C32">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>231</v>
-      </c>
-      <c r="B33">
-        <v>1987</v>
-      </c>
-      <c r="C33">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>231</v>
-      </c>
-      <c r="B34">
-        <v>1986</v>
-      </c>
-      <c r="C34">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>231</v>
-      </c>
-      <c r="B35">
-        <v>1985</v>
-      </c>
-      <c r="C35">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B36">
-        <v>1984</v>
-      </c>
-      <c r="C36">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>231</v>
-      </c>
-      <c r="B37">
-        <v>1983</v>
-      </c>
-      <c r="C37">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>231</v>
-      </c>
-      <c r="B38">
-        <v>1982</v>
-      </c>
-      <c r="C38">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>231</v>
-      </c>
-      <c r="B39">
-        <v>1981</v>
-      </c>
-      <c r="C39">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>231</v>
-      </c>
-      <c r="B40">
-        <v>1980</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B102"/>
   <sheetViews>
@@ -79767,12 +79309,12 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2">
         <v>97</v>
@@ -79780,7 +79322,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3">
         <v>95</v>
@@ -79788,7 +79330,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4">
         <v>97</v>
@@ -79796,7 +79338,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5">
         <v>95</v>
@@ -79804,7 +79346,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6">
         <v>99</v>
@@ -79812,7 +79354,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B7">
         <v>99</v>
@@ -79820,7 +79362,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B8">
         <v>97</v>
@@ -79828,7 +79370,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B9">
         <v>91</v>
@@ -79836,7 +79378,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B10">
         <v>78</v>
@@ -79844,7 +79386,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11">
         <v>93</v>
@@ -79852,7 +79394,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12">
         <v>83</v>
@@ -79860,7 +79402,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13">
         <v>87</v>
@@ -79868,7 +79410,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14">
         <v>99</v>
@@ -79876,7 +79418,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B15">
         <v>99</v>
@@ -79884,7 +79426,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16">
         <v>95</v>
@@ -79892,7 +79434,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17">
         <v>97</v>
@@ -79900,7 +79442,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B18">
         <v>94</v>
@@ -79908,7 +79450,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19">
         <v>96</v>
@@ -79916,7 +79458,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B20">
         <v>98</v>
@@ -79924,7 +79466,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21">
         <v>96</v>
@@ -79932,7 +79474,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22">
         <v>97</v>
@@ -79940,7 +79482,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B23">
         <v>96</v>
@@ -79948,7 +79490,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B24">
         <v>90</v>
@@ -79956,7 +79498,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B25">
         <v>92</v>
@@ -79964,7 +79506,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B26">
         <v>87</v>
@@ -79972,7 +79514,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B27">
         <v>87</v>
@@ -79980,7 +79522,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B28">
         <v>74</v>
@@ -79988,7 +79530,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B29">
         <v>81</v>
@@ -79996,7 +79538,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B30">
         <v>87</v>
@@ -80004,7 +79546,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B31">
         <v>86</v>
@@ -80012,7 +79554,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -80020,7 +79562,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -80028,7 +79570,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -80036,7 +79578,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -80044,7 +79586,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -80052,7 +79594,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -80060,7 +79602,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -80068,7 +79610,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -80076,7 +79618,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -80084,7 +79626,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -80092,7 +79634,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -80100,7 +79642,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -80108,7 +79650,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -80116,7 +79658,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -80124,7 +79666,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -80132,7 +79674,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -80140,7 +79682,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -80148,7 +79690,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -80156,7 +79698,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -80164,7 +79706,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -80172,7 +79714,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -80180,7 +79722,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -80188,7 +79730,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -80196,7 +79738,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -80204,7 +79746,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -80212,7 +79754,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -80220,7 +79762,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -80228,7 +79770,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -80236,7 +79778,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -80244,7 +79786,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -80252,7 +79794,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -80260,7 +79802,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -80268,7 +79810,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -80276,7 +79818,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -80284,7 +79826,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -80292,7 +79834,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -80300,7 +79842,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -80308,7 +79850,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -80316,7 +79858,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -80324,7 +79866,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -80332,7 +79874,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -80340,7 +79882,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -80348,7 +79890,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -80356,7 +79898,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -80364,7 +79906,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -80372,7 +79914,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -80380,7 +79922,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -80388,7 +79930,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -80396,7 +79938,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -80404,7 +79946,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -80412,7 +79954,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -80420,7 +79962,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -80428,7 +79970,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -80436,7 +79978,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -80444,7 +79986,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -80452,7 +79994,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -80460,7 +80002,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -80468,7 +80010,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -80476,7 +80018,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -80484,7 +80026,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -80492,7 +80034,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -80500,7 +80042,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -80508,7 +80050,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -80516,7 +80058,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -80524,7 +80066,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -80532,7 +80074,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -80540,7 +80082,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -80548,7 +80090,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -80556,7 +80098,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -80564,7 +80106,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -80572,10 +80114,465 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B102">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2">
+        <v>2018</v>
+      </c>
+      <c r="C2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3">
+        <v>2017</v>
+      </c>
+      <c r="C3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4">
+        <v>2016</v>
+      </c>
+      <c r="C4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6">
+        <v>2014</v>
+      </c>
+      <c r="C6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7">
+        <v>2013</v>
+      </c>
+      <c r="C7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8">
+        <v>2012</v>
+      </c>
+      <c r="C8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9">
+        <v>2011</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10">
+        <v>2010</v>
+      </c>
+      <c r="C10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11">
+        <v>2009</v>
+      </c>
+      <c r="C11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12">
+        <v>2008</v>
+      </c>
+      <c r="C12">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13">
+        <v>2007</v>
+      </c>
+      <c r="C13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14">
+        <v>2006</v>
+      </c>
+      <c r="C14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15">
+        <v>2005</v>
+      </c>
+      <c r="C15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16">
+        <v>2004</v>
+      </c>
+      <c r="C16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17">
+        <v>2003</v>
+      </c>
+      <c r="C17">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18">
+        <v>2002</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19">
+        <v>2001</v>
+      </c>
+      <c r="C19">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20">
+        <v>2000</v>
+      </c>
+      <c r="C20">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21">
+        <v>1999</v>
+      </c>
+      <c r="C21">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22">
+        <v>1998</v>
+      </c>
+      <c r="C22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23">
+        <v>1997</v>
+      </c>
+      <c r="C23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24">
+        <v>1996</v>
+      </c>
+      <c r="C24">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25">
+        <v>1995</v>
+      </c>
+      <c r="C25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26">
+        <v>1994</v>
+      </c>
+      <c r="C26">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27">
+        <v>1993</v>
+      </c>
+      <c r="C27">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28">
+        <v>1992</v>
+      </c>
+      <c r="C28">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29">
+        <v>1991</v>
+      </c>
+      <c r="C29">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30">
+        <v>1990</v>
+      </c>
+      <c r="C30">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>230</v>
+      </c>
+      <c r="B31">
+        <v>1989</v>
+      </c>
+      <c r="C31">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32">
+        <v>1988</v>
+      </c>
+      <c r="C32">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33">
+        <v>1987</v>
+      </c>
+      <c r="C33">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B34">
+        <v>1986</v>
+      </c>
+      <c r="C34">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35">
+        <v>1985</v>
+      </c>
+      <c r="C35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>230</v>
+      </c>
+      <c r="B36">
+        <v>1984</v>
+      </c>
+      <c r="C36">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B37">
+        <v>1983</v>
+      </c>
+      <c r="C37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38">
+        <v>1982</v>
+      </c>
+      <c r="C38">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39">
+        <v>1981</v>
+      </c>
+      <c r="C39">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>230</v>
+      </c>
+      <c r="B40">
+        <v>1980</v>
       </c>
     </row>
   </sheetData>
@@ -80954,7 +80951,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add non-tb symptomatic population seeking care
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8113" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8114" uniqueCount="335">
   <si>
     <t>Name:</t>
   </si>
@@ -1057,6 +1057,9 @@
   <si>
     <t>bcg_coverage</t>
   </si>
+  <si>
+    <t>presump_testing</t>
+  </si>
 </sst>
 </file>
 
@@ -80129,7 +80132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -80948,10 +80951,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -81438,6 +81441,14 @@
       </c>
       <c r="B60" s="34">
         <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="B61" s="34">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split mdr-tb deaths, include tb deaths on treatment
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8114" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8117" uniqueCount="339">
   <si>
     <t>Name:</t>
   </si>
@@ -569,9 +569,6 @@
     <t>prop_pulm_10yr</t>
   </si>
   <si>
-    <t>mortality_cotrim</t>
-  </si>
-  <si>
     <t>rr_tb_bcg</t>
   </si>
   <si>
@@ -1059,6 +1056,21 @@
   </si>
   <si>
     <t>presump_testing</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>mort_cotrim</t>
+  </si>
+  <si>
+    <t>mort_tx</t>
   </si>
 </sst>
 </file>
@@ -4935,7 +4947,7 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -78282,52 +78294,52 @@
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
         <v>219</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I1" t="s">
         <v>220</v>
       </c>
-      <c r="F1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>221</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>222</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>223</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>224</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>225</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>226</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>227</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>228</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -79312,12 +79324,12 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B2">
         <v>97</v>
@@ -79325,7 +79337,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B3">
         <v>95</v>
@@ -79333,7 +79345,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4">
         <v>97</v>
@@ -79341,7 +79353,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B5">
         <v>95</v>
@@ -79349,7 +79361,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B6">
         <v>99</v>
@@ -79357,7 +79369,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7">
         <v>99</v>
@@ -79365,7 +79377,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B8">
         <v>97</v>
@@ -79373,7 +79385,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9">
         <v>91</v>
@@ -79381,7 +79393,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10">
         <v>78</v>
@@ -79389,7 +79401,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11">
         <v>93</v>
@@ -79397,7 +79409,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B12">
         <v>83</v>
@@ -79405,7 +79417,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13">
         <v>87</v>
@@ -79413,7 +79425,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14">
         <v>99</v>
@@ -79421,7 +79433,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15">
         <v>99</v>
@@ -79429,7 +79441,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B16">
         <v>95</v>
@@ -79437,7 +79449,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B17">
         <v>97</v>
@@ -79445,7 +79457,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B18">
         <v>94</v>
@@ -79453,7 +79465,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B19">
         <v>96</v>
@@ -79461,7 +79473,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B20">
         <v>98</v>
@@ -79469,7 +79481,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21">
         <v>96</v>
@@ -79477,7 +79489,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B22">
         <v>97</v>
@@ -79485,7 +79497,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B23">
         <v>96</v>
@@ -79493,7 +79505,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B24">
         <v>90</v>
@@ -79501,7 +79513,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B25">
         <v>92</v>
@@ -79509,7 +79521,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B26">
         <v>87</v>
@@ -79517,7 +79529,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B27">
         <v>87</v>
@@ -79525,7 +79537,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B28">
         <v>74</v>
@@ -79533,7 +79545,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B29">
         <v>81</v>
@@ -79541,7 +79553,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B30">
         <v>87</v>
@@ -79549,7 +79561,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B31">
         <v>86</v>
@@ -79557,7 +79569,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -79565,7 +79577,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -79573,7 +79585,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -79581,7 +79593,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -79589,7 +79601,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -79597,7 +79609,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -79605,7 +79617,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -79613,7 +79625,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -79621,7 +79633,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -79629,7 +79641,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -79637,7 +79649,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -79645,7 +79657,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -79653,7 +79665,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -79661,7 +79673,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -79669,7 +79681,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -79677,7 +79689,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -79685,7 +79697,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -79693,7 +79705,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -79701,7 +79713,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -79709,7 +79721,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -79717,7 +79729,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -79725,7 +79737,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -79733,7 +79745,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -79741,7 +79753,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -79749,7 +79761,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -79757,7 +79769,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -79765,7 +79777,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -79773,7 +79785,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -79781,7 +79793,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -79789,7 +79801,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -79797,7 +79809,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -79805,7 +79817,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -79813,7 +79825,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -79821,7 +79833,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -79829,7 +79841,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -79837,7 +79849,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -79845,7 +79857,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -79853,7 +79865,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -79861,7 +79873,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -79869,7 +79881,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -79877,7 +79889,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -79885,7 +79897,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -79893,7 +79905,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -79901,7 +79913,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -79909,7 +79921,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -79917,7 +79929,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -79925,7 +79937,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -79933,7 +79945,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -79941,7 +79953,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -79949,7 +79961,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -79957,7 +79969,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -79965,7 +79977,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -79973,7 +79985,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -79981,7 +79993,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -79989,7 +80001,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -79997,7 +80009,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -80005,7 +80017,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -80013,7 +80025,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -80021,7 +80033,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -80029,7 +80041,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -80037,7 +80049,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -80045,7 +80057,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -80053,7 +80065,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -80061,7 +80073,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -80069,7 +80081,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -80077,7 +80089,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -80085,7 +80097,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -80093,7 +80105,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -80101,7 +80113,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -80109,7 +80121,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -80117,7 +80129,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -80143,18 +80155,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2">
         <v>2018</v>
@@ -80165,7 +80177,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3">
         <v>2017</v>
@@ -80176,7 +80188,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4">
         <v>2016</v>
@@ -80187,7 +80199,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5">
         <v>2015</v>
@@ -80198,7 +80210,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6">
         <v>2014</v>
@@ -80209,7 +80221,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7">
         <v>2013</v>
@@ -80220,7 +80232,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8">
         <v>2012</v>
@@ -80231,7 +80243,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>2011</v>
@@ -80242,7 +80254,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10">
         <v>2010</v>
@@ -80253,7 +80265,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11">
         <v>2009</v>
@@ -80264,7 +80276,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12">
         <v>2008</v>
@@ -80275,7 +80287,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13">
         <v>2007</v>
@@ -80286,7 +80298,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14">
         <v>2006</v>
@@ -80297,7 +80309,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B15">
         <v>2005</v>
@@ -80308,7 +80320,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16">
         <v>2004</v>
@@ -80319,7 +80331,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B17">
         <v>2003</v>
@@ -80330,7 +80342,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B18">
         <v>2002</v>
@@ -80341,7 +80353,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B19">
         <v>2001</v>
@@ -80352,7 +80364,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B20">
         <v>2000</v>
@@ -80363,7 +80375,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B21">
         <v>1999</v>
@@ -80374,7 +80386,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B22">
         <v>1998</v>
@@ -80385,7 +80397,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23">
         <v>1997</v>
@@ -80396,7 +80408,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24">
         <v>1996</v>
@@ -80407,7 +80419,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25">
         <v>1995</v>
@@ -80418,7 +80430,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26">
         <v>1994</v>
@@ -80429,7 +80441,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27">
         <v>1993</v>
@@ -80440,7 +80452,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B28">
         <v>1992</v>
@@ -80451,7 +80463,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B29">
         <v>1991</v>
@@ -80462,7 +80474,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30">
         <v>1990</v>
@@ -80473,7 +80485,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B31">
         <v>1989</v>
@@ -80484,7 +80496,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B32">
         <v>1988</v>
@@ -80495,7 +80507,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33">
         <v>1987</v>
@@ -80506,7 +80518,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B34">
         <v>1986</v>
@@ -80517,7 +80529,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B35">
         <v>1985</v>
@@ -80528,7 +80540,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B36">
         <v>1984</v>
@@ -80539,7 +80551,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B37">
         <v>1983</v>
@@ -80550,7 +80562,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38">
         <v>1982</v>
@@ -80561,7 +80573,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B39">
         <v>1981</v>
@@ -80572,7 +80584,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B40">
         <v>1980</v>
@@ -80951,10 +80963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -80963,15 +80975,21 @@
     <col min="2" max="2" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+      <c r="C1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>155</v>
       </c>
@@ -80979,7 +80997,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>156</v>
       </c>
@@ -80987,7 +81005,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>157</v>
       </c>
@@ -80995,7 +81013,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>68</v>
       </c>
@@ -81003,7 +81021,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>61</v>
       </c>
@@ -81011,7 +81029,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>158</v>
       </c>
@@ -81019,7 +81037,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>159</v>
       </c>
@@ -81027,7 +81045,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>133</v>
       </c>
@@ -81035,7 +81053,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>134</v>
       </c>
@@ -81043,7 +81061,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>135</v>
       </c>
@@ -81051,15 +81069,15 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="28">
         <v>4.7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>60</v>
       </c>
@@ -81067,7 +81085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>160</v>
       </c>
@@ -81075,7 +81093,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>161</v>
       </c>
@@ -81083,7 +81101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>162</v>
       </c>
@@ -81093,7 +81111,7 @@
     </row>
     <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="28">
         <v>0.05</v>
@@ -81101,7 +81119,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="28">
         <v>0.02</v>
@@ -81125,7 +81143,7 @@
     </row>
     <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B21" s="28">
         <v>8.2500000000000004E-3</v>
@@ -81221,233 +81239,241 @@
     </row>
     <row r="33" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
-        <v>171</v>
+        <v>337</v>
       </c>
       <c r="B33" s="28">
         <v>0.35</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="B34" s="25">
-        <v>0.42</v>
+      <c r="A34" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="B34" s="28">
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B35" s="25">
-        <v>5</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="B36" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="25">
         <v>26.06</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B37" s="25">
-        <v>0.35</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B38" s="25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="25">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="B39" s="29">
-        <v>0.62</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B40" s="29">
-        <v>0.4</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="28">
-        <v>3</v>
+        <v>176</v>
+      </c>
+      <c r="B41" s="29">
+        <v>0.4</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42" s="28">
-        <v>2.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="28">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B44" s="28">
         <v>2.6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B44" s="25">
-        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B45" s="25">
-        <v>548</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B46" s="25">
-        <v>0.4</v>
+        <v>548</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B47" s="25">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B48" s="25">
-        <v>0.68</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" s="25">
-        <v>0.86</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B50" s="25">
-        <v>0.76</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B51" s="25">
-        <v>0.63</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="B52" s="25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="B53" s="25">
+      <c r="B54" s="25">
         <v>0.82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="B54" s="25">
-        <v>0.81</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B55" s="25">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B56" s="25">
-        <v>0.61</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B57" s="25">
-        <v>0.78500000000000003</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B58" s="25">
-        <v>0.78200000000000003</v>
+        <v>0.78500000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="23" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B59" s="25">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="25">
         <v>0.84399999999999997</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="B60" s="34">
-        <v>0.75</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>334</v>
+        <v>214</v>
       </c>
       <c r="B61" s="34">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="B62" s="34">
         <v>1E-3</v>
       </c>
     </row>
@@ -81472,57 +81498,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -81560,7 +81586,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2">
         <v>0.7</v>
@@ -81571,7 +81597,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3">
         <v>0.74</v>
@@ -81582,7 +81608,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>0.91</v>
@@ -81593,7 +81619,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C5">
         <v>0.91</v>
@@ -81604,7 +81630,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6">
         <v>0.91</v>
@@ -81615,7 +81641,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7">
         <v>0.89</v>
@@ -81626,7 +81652,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8">
         <v>0.89</v>
@@ -81637,7 +81663,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9">
         <v>0.89</v>
@@ -81648,7 +81674,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10">
         <v>0.89</v>
@@ -81659,7 +81685,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11">
         <v>0.89</v>
@@ -81670,7 +81696,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12">
         <v>0.99</v>
@@ -81681,7 +81707,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13">
         <v>0.99</v>
@@ -81692,7 +81718,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C14">
         <v>0.99</v>
@@ -81703,7 +81729,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15">
         <v>0.99</v>
@@ -81714,7 +81740,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16">
         <v>0.99</v>
@@ -81725,7 +81751,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17">
         <v>0.8</v>
@@ -81736,7 +81762,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18">
         <v>0.8</v>
@@ -81747,7 +81773,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C19">
         <v>0.8</v>
@@ -81758,7 +81784,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C20">
         <v>0.8</v>
@@ -81769,7 +81795,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21">
         <v>0.8</v>
@@ -81780,7 +81806,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22">
         <v>0.8</v>
@@ -81791,7 +81817,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C23">
         <v>0.8</v>
@@ -81802,7 +81828,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24">
         <v>0.8</v>
@@ -81813,7 +81839,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C25">
         <v>0.8</v>
@@ -81824,7 +81850,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C26">
         <v>0.8</v>
@@ -81835,7 +81861,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27">
         <v>0.8</v>
@@ -81846,7 +81872,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28">
         <v>0.8</v>
@@ -81857,7 +81883,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29">
         <v>0.8</v>
@@ -81868,7 +81894,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30">
         <v>0.8</v>
@@ -81879,7 +81905,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31">
         <v>0.8</v>
@@ -81890,7 +81916,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32">
         <v>0.8</v>
@@ -81901,7 +81927,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33">
         <v>0.8</v>
@@ -81912,7 +81938,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C34">
         <v>0.8</v>
@@ -81923,7 +81949,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C35">
         <v>0.8</v>
@@ -81934,7 +81960,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C36">
         <v>0.8</v>
@@ -81945,7 +81971,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37">
         <v>0.8</v>
@@ -81956,7 +81982,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C38">
         <v>0.8</v>
@@ -81967,7 +81993,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C39">
         <v>0.8</v>
@@ -81978,7 +82004,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C40">
         <v>0.8</v>
@@ -81989,7 +82015,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C41">
         <v>0.8</v>
@@ -82000,7 +82026,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C42">
         <v>0.8</v>
@@ -82011,7 +82037,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43">
         <v>0.8</v>
@@ -82022,7 +82048,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C44">
         <v>0.8</v>
@@ -82033,7 +82059,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C45">
         <v>0.8</v>
@@ -82044,7 +82070,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C46">
         <v>0.8</v>
@@ -82055,7 +82081,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C47">
         <v>0.8</v>
@@ -82066,7 +82092,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C48">
         <v>0.8</v>
@@ -82077,7 +82103,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C49">
         <v>0.8</v>
@@ -82088,7 +82114,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50">
         <v>0.8</v>
@@ -82099,7 +82125,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51">
         <v>0.8</v>
@@ -82110,7 +82136,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C52">
         <v>0.8</v>
@@ -82121,7 +82147,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C53">
         <v>0.8</v>
@@ -82132,7 +82158,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C54">
         <v>0.8</v>
@@ -82143,7 +82169,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C55">
         <v>0.8</v>
@@ -82154,7 +82180,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C56">
         <v>0.8</v>
@@ -82165,7 +82191,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C57">
         <v>0.8</v>
@@ -82176,7 +82202,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C58">
         <v>0.8</v>
@@ -82187,7 +82213,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C59">
         <v>0.8</v>
@@ -82198,7 +82224,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C60">
         <v>0.8</v>
@@ -82209,7 +82235,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C61">
         <v>0.8</v>
@@ -82220,7 +82246,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C62">
         <v>0.8</v>
@@ -82231,7 +82257,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C63">
         <v>0.8</v>
@@ -82242,7 +82268,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C64">
         <v>0.8</v>
@@ -82253,7 +82279,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C65">
         <v>0.8</v>
@@ -82264,7 +82290,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C66">
         <v>0.8</v>
@@ -82275,7 +82301,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C67">
         <v>0.8</v>
@@ -82286,7 +82312,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C68">
         <v>0.8</v>
@@ -82297,7 +82323,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69">
         <v>0.8</v>
@@ -82308,7 +82334,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70">
         <v>0.8</v>
@@ -82319,7 +82345,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C71">
         <v>0.8</v>
@@ -82330,7 +82356,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C72">
         <v>0.8</v>
@@ -82341,7 +82367,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C73">
         <v>0.8</v>
@@ -82352,7 +82378,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C74">
         <v>0.8</v>
@@ -82363,7 +82389,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C75">
         <v>0.8</v>
@@ -82374,7 +82400,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C76">
         <v>0.8</v>
@@ -82385,7 +82411,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C77">
         <v>0.8</v>
@@ -82396,7 +82422,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78">
         <v>0.8</v>
@@ -82407,7 +82433,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C79">
         <v>0.8</v>
@@ -82418,7 +82444,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C80">
         <v>0.8</v>
@@ -82429,7 +82455,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C81">
         <v>0.8</v>
@@ -82440,7 +82466,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C82">
         <v>0.8</v>
@@ -82451,7 +82477,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C83">
         <v>0.8</v>
@@ -82462,7 +82488,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C84">
         <v>0.8</v>
@@ -82473,7 +82499,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C85">
         <v>0.8</v>
@@ -82484,7 +82510,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86">
         <v>0.8</v>
@@ -82495,7 +82521,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C87">
         <v>0.8</v>
@@ -82506,7 +82532,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C88">
         <v>0.8</v>
@@ -82517,7 +82543,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C89">
         <v>0.8</v>
@@ -82528,7 +82554,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C90">
         <v>0.8</v>
@@ -82539,7 +82565,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C91">
         <v>0.8</v>
@@ -82550,7 +82576,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C92">
         <v>0.8</v>
@@ -82561,7 +82587,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C93">
         <v>0.8</v>
@@ -82572,7 +82598,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C94">
         <v>0.8</v>
@@ -82583,7 +82609,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C95">
         <v>0.8</v>
@@ -82594,7 +82620,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C96">
         <v>0.8</v>
@@ -82605,7 +82631,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C97">
         <v>0.8</v>
@@ -82616,7 +82642,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C98">
         <v>0.8</v>
@@ -82627,7 +82653,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C99">
         <v>0.8</v>
@@ -82638,7 +82664,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C100">
         <v>0.8</v>
@@ -82649,7 +82675,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C101">
         <v>0.8</v>
@@ -82660,7 +82686,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C102">
         <v>0.8</v>
@@ -82671,7 +82697,7 @@
         <v>0</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C103">
         <v>0.5</v>
@@ -82682,7 +82708,7 @@
         <v>1</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C104">
         <v>0.5</v>
@@ -82693,7 +82719,7 @@
         <v>2</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C105">
         <v>0.5</v>
@@ -82704,7 +82730,7 @@
         <v>3</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C106">
         <v>0.5</v>
@@ -82715,7 +82741,7 @@
         <v>4</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C107">
         <v>0.5</v>
@@ -82726,7 +82752,7 @@
         <v>5</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C108">
         <v>0.5</v>
@@ -82737,7 +82763,7 @@
         <v>6</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C109">
         <v>0.5</v>
@@ -82748,7 +82774,7 @@
         <v>7</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C110">
         <v>0.5</v>
@@ -82759,7 +82785,7 @@
         <v>8</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C111">
         <v>0.5</v>
@@ -82770,7 +82796,7 @@
         <v>9</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C112">
         <v>0.5</v>
@@ -82781,7 +82807,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C113">
         <v>0.5</v>
@@ -82792,7 +82818,7 @@
         <v>11</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C114">
         <v>0.5</v>
@@ -82803,7 +82829,7 @@
         <v>12</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C115">
         <v>0.5</v>
@@ -82814,7 +82840,7 @@
         <v>13</v>
       </c>
       <c r="B116" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C116">
         <v>0.5</v>
@@ -82825,7 +82851,7 @@
         <v>14</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C117">
         <v>0.5</v>
@@ -82836,7 +82862,7 @@
         <v>15</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C118">
         <v>0.5</v>
@@ -82847,7 +82873,7 @@
         <v>16</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C119">
         <v>0.5</v>
@@ -82858,7 +82884,7 @@
         <v>17</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C120">
         <v>0.5</v>
@@ -82869,7 +82895,7 @@
         <v>18</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C121">
         <v>0.5</v>
@@ -82880,7 +82906,7 @@
         <v>19</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C122">
         <v>0.5</v>
@@ -82891,7 +82917,7 @@
         <v>20</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C123">
         <v>0.5</v>
@@ -82902,7 +82928,7 @@
         <v>21</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C124">
         <v>0.5</v>
@@ -82913,7 +82939,7 @@
         <v>22</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C125">
         <v>0.5</v>
@@ -82924,7 +82950,7 @@
         <v>23</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C126">
         <v>0.5</v>
@@ -82935,7 +82961,7 @@
         <v>24</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C127">
         <v>0.5</v>
@@ -82946,7 +82972,7 @@
         <v>25</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C128">
         <v>0.5</v>
@@ -82957,7 +82983,7 @@
         <v>26</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C129">
         <v>0.5</v>
@@ -82968,7 +82994,7 @@
         <v>27</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C130">
         <v>0.5</v>
@@ -82979,7 +83005,7 @@
         <v>28</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C131">
         <v>0.5</v>
@@ -82990,7 +83016,7 @@
         <v>29</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C132">
         <v>0.5</v>
@@ -83001,7 +83027,7 @@
         <v>30</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C133">
         <v>0.5</v>
@@ -83012,7 +83038,7 @@
         <v>31</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C134">
         <v>0.5</v>
@@ -83023,7 +83049,7 @@
         <v>32</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C135">
         <v>0.5</v>
@@ -83034,7 +83060,7 @@
         <v>33</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C136">
         <v>0.5</v>
@@ -83045,7 +83071,7 @@
         <v>34</v>
       </c>
       <c r="B137" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C137">
         <v>0.5</v>
@@ -83056,7 +83082,7 @@
         <v>35</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C138">
         <v>0.5</v>
@@ -83067,7 +83093,7 @@
         <v>36</v>
       </c>
       <c r="B139" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C139">
         <v>0.5</v>
@@ -83078,7 +83104,7 @@
         <v>37</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C140">
         <v>0.5</v>
@@ -83089,7 +83115,7 @@
         <v>38</v>
       </c>
       <c r="B141" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C141">
         <v>0.5</v>
@@ -83100,7 +83126,7 @@
         <v>39</v>
       </c>
       <c r="B142" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C142">
         <v>0.5</v>
@@ -83111,7 +83137,7 @@
         <v>40</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C143">
         <v>0.5</v>
@@ -83122,7 +83148,7 @@
         <v>41</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C144">
         <v>0.5</v>
@@ -83133,7 +83159,7 @@
         <v>42</v>
       </c>
       <c r="B145" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C145">
         <v>0.5</v>
@@ -83144,7 +83170,7 @@
         <v>43</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C146">
         <v>0.5</v>
@@ -83155,7 +83181,7 @@
         <v>44</v>
       </c>
       <c r="B147" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C147">
         <v>0.5</v>
@@ -83166,7 +83192,7 @@
         <v>45</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C148">
         <v>0.5</v>
@@ -83177,7 +83203,7 @@
         <v>46</v>
       </c>
       <c r="B149" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C149">
         <v>0.5</v>
@@ -83188,7 +83214,7 @@
         <v>47</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C150">
         <v>0.5</v>
@@ -83199,7 +83225,7 @@
         <v>48</v>
       </c>
       <c r="B151" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C151">
         <v>0.5</v>
@@ -83210,7 +83236,7 @@
         <v>49</v>
       </c>
       <c r="B152" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C152">
         <v>0.5</v>
@@ -83221,7 +83247,7 @@
         <v>50</v>
       </c>
       <c r="B153" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C153">
         <v>0.5</v>
@@ -83232,7 +83258,7 @@
         <v>51</v>
       </c>
       <c r="B154" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C154">
         <v>0.5</v>
@@ -83243,7 +83269,7 @@
         <v>52</v>
       </c>
       <c r="B155" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C155">
         <v>0.5</v>
@@ -83254,7 +83280,7 @@
         <v>53</v>
       </c>
       <c r="B156" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C156">
         <v>0.5</v>
@@ -83265,7 +83291,7 @@
         <v>54</v>
       </c>
       <c r="B157" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C157">
         <v>0.5</v>
@@ -83276,7 +83302,7 @@
         <v>55</v>
       </c>
       <c r="B158" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C158">
         <v>0.5</v>
@@ -83287,7 +83313,7 @@
         <v>56</v>
       </c>
       <c r="B159" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C159">
         <v>0.5</v>
@@ -83298,7 +83324,7 @@
         <v>57</v>
       </c>
       <c r="B160" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C160">
         <v>0.5</v>
@@ -83309,7 +83335,7 @@
         <v>58</v>
       </c>
       <c r="B161" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C161">
         <v>0.5</v>
@@ -83320,7 +83346,7 @@
         <v>59</v>
       </c>
       <c r="B162" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C162">
         <v>0.5</v>
@@ -83331,7 +83357,7 @@
         <v>60</v>
       </c>
       <c r="B163" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C163">
         <v>0.5</v>
@@ -83342,7 +83368,7 @@
         <v>61</v>
       </c>
       <c r="B164" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C164">
         <v>0.5</v>
@@ -83353,7 +83379,7 @@
         <v>62</v>
       </c>
       <c r="B165" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C165">
         <v>0.5</v>
@@ -83364,7 +83390,7 @@
         <v>63</v>
       </c>
       <c r="B166" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C166">
         <v>0.5</v>
@@ -83375,7 +83401,7 @@
         <v>64</v>
       </c>
       <c r="B167" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C167">
         <v>0.5</v>
@@ -83386,7 +83412,7 @@
         <v>65</v>
       </c>
       <c r="B168" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C168">
         <v>0.5</v>
@@ -83397,7 +83423,7 @@
         <v>66</v>
       </c>
       <c r="B169" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C169">
         <v>0.5</v>
@@ -83408,7 +83434,7 @@
         <v>67</v>
       </c>
       <c r="B170" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C170">
         <v>0.5</v>
@@ -83419,7 +83445,7 @@
         <v>68</v>
       </c>
       <c r="B171" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C171">
         <v>0.5</v>
@@ -83430,7 +83456,7 @@
         <v>69</v>
       </c>
       <c r="B172" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C172">
         <v>0.5</v>
@@ -83441,7 +83467,7 @@
         <v>70</v>
       </c>
       <c r="B173" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C173">
         <v>0.5</v>
@@ -83452,7 +83478,7 @@
         <v>71</v>
       </c>
       <c r="B174" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C174">
         <v>0.5</v>
@@ -83463,7 +83489,7 @@
         <v>72</v>
       </c>
       <c r="B175" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C175">
         <v>0.5</v>
@@ -83474,7 +83500,7 @@
         <v>73</v>
       </c>
       <c r="B176" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C176">
         <v>0.5</v>
@@ -83485,7 +83511,7 @@
         <v>74</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C177">
         <v>0.5</v>
@@ -83496,7 +83522,7 @@
         <v>75</v>
       </c>
       <c r="B178" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C178">
         <v>0.5</v>
@@ -83507,7 +83533,7 @@
         <v>76</v>
       </c>
       <c r="B179" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C179">
         <v>0.5</v>
@@ -83518,7 +83544,7 @@
         <v>77</v>
       </c>
       <c r="B180" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C180">
         <v>0.5</v>
@@ -83529,7 +83555,7 @@
         <v>78</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C181">
         <v>0.5</v>
@@ -83540,7 +83566,7 @@
         <v>79</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C182">
         <v>0.5</v>
@@ -83551,7 +83577,7 @@
         <v>80</v>
       </c>
       <c r="B183" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C183">
         <v>0.5</v>
@@ -83562,7 +83588,7 @@
         <v>81</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C184">
         <v>0.5</v>
@@ -83573,7 +83599,7 @@
         <v>82</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C185">
         <v>0.5</v>
@@ -83584,7 +83610,7 @@
         <v>83</v>
       </c>
       <c r="B186" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C186">
         <v>0.5</v>
@@ -83595,7 +83621,7 @@
         <v>84</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C187">
         <v>0.5</v>
@@ -83606,7 +83632,7 @@
         <v>85</v>
       </c>
       <c r="B188" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C188">
         <v>0.5</v>
@@ -83617,7 +83643,7 @@
         <v>86</v>
       </c>
       <c r="B189" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C189">
         <v>0.5</v>
@@ -83628,7 +83654,7 @@
         <v>87</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C190">
         <v>0.5</v>
@@ -83639,7 +83665,7 @@
         <v>88</v>
       </c>
       <c r="B191" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C191">
         <v>0.5</v>
@@ -83650,7 +83676,7 @@
         <v>89</v>
       </c>
       <c r="B192" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C192">
         <v>0.5</v>
@@ -83661,7 +83687,7 @@
         <v>90</v>
       </c>
       <c r="B193" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C193">
         <v>0.5</v>
@@ -83672,7 +83698,7 @@
         <v>91</v>
       </c>
       <c r="B194" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C194">
         <v>0.5</v>
@@ -83683,7 +83709,7 @@
         <v>92</v>
       </c>
       <c r="B195" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C195">
         <v>0.5</v>
@@ -83694,7 +83720,7 @@
         <v>93</v>
       </c>
       <c r="B196" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C196">
         <v>0.5</v>
@@ -83705,7 +83731,7 @@
         <v>94</v>
       </c>
       <c r="B197" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C197">
         <v>0.5</v>
@@ -83716,7 +83742,7 @@
         <v>95</v>
       </c>
       <c r="B198" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C198">
         <v>0.5</v>
@@ -83727,7 +83753,7 @@
         <v>96</v>
       </c>
       <c r="B199" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C199">
         <v>0.5</v>
@@ -83738,7 +83764,7 @@
         <v>97</v>
       </c>
       <c r="B200" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C200">
         <v>0.5</v>
@@ -83749,7 +83775,7 @@
         <v>98</v>
       </c>
       <c r="B201" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C201">
         <v>0.5</v>
@@ -83760,7 +83786,7 @@
         <v>99</v>
       </c>
       <c r="B202" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C202">
         <v>0.5</v>
@@ -83771,7 +83797,7 @@
         <v>100</v>
       </c>
       <c r="B203" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C203">
         <v>0.5</v>
@@ -84152,7 +84178,7 @@
         <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
         <v>150</v>
@@ -84161,7 +84187,7 @@
         <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G1" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
new latent cases distributed using district-level foi
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -74375,8 +74375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -82565,7 +82565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
edits to prevalence outputs
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_TB.xlsx
+++ b/resources/ResourceFile_TB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="14835" windowHeight="9360" tabRatio="731" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="16" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="315">
   <si>
     <t>Age</t>
   </si>
@@ -983,6 +983,15 @@
   </si>
   <si>
     <t>case_detection_rate_upper</t>
+  </si>
+  <si>
+    <t>all_cases</t>
+  </si>
+  <si>
+    <t>general_prob</t>
+  </si>
+  <si>
+    <t>whole_pop</t>
   </si>
 </sst>
 </file>
@@ -4516,9 +4525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T1" sqref="T1"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9786,10 +9795,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9799,7 +9808,7 @@
     <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>294</v>
       </c>
@@ -9815,8 +9824,17 @@
       <c r="E1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -9834,8 +9852,19 @@
         <f>C2/D2</f>
         <v>3.5654080145262434E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>50000</v>
+      </c>
+      <c r="G2">
+        <f>SUM(D2:D33)</f>
+        <v>17563749</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2</f>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -9853,8 +9882,18 @@
         <f t="shared" ref="E3:E33" si="1">C3/D3</f>
         <v>3.4639422011435664E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>50000</v>
+      </c>
+      <c r="G3">
+        <v>17563749</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H33" si="2">F3/G3</f>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>283</v>
       </c>
@@ -9872,8 +9911,18 @@
         <f t="shared" si="1"/>
         <v>1.9531054751931864E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>50000</v>
+      </c>
+      <c r="G4">
+        <v>17563749</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -9891,8 +9940,18 @@
         <f t="shared" si="1"/>
         <v>2.7679197568905795E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>50000</v>
+      </c>
+      <c r="G5">
+        <v>17563749</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -9910,8 +9969,18 @@
         <f t="shared" si="1"/>
         <v>4.3796847635726799E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>50000</v>
+      </c>
+      <c r="G6">
+        <v>17563749</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>290</v>
       </c>
@@ -9929,8 +9998,18 @@
         <f t="shared" si="1"/>
         <v>6.653130546935857E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>50000</v>
+      </c>
+      <c r="G7">
+        <v>17563749</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -9948,8 +10027,18 @@
         <f t="shared" si="1"/>
         <v>1.8819716030593176E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>50000</v>
+      </c>
+      <c r="G8">
+        <v>17563749</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>277</v>
       </c>
@@ -9967,8 +10056,18 @@
         <f t="shared" si="1"/>
         <v>2.0231202649860403E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>50000</v>
+      </c>
+      <c r="G9">
+        <v>17563749</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>289</v>
       </c>
@@ -9986,8 +10085,18 @@
         <f t="shared" si="1"/>
         <v>4.2818633091160126E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>50000</v>
+      </c>
+      <c r="G10">
+        <v>17563749</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>279</v>
       </c>
@@ -10005,8 +10114,18 @@
         <f t="shared" si="1"/>
         <v>1.8541959041607301E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>50000</v>
+      </c>
+      <c r="G11">
+        <v>17563749</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -10024,8 +10143,18 @@
         <f t="shared" si="1"/>
         <v>0.10759275831210849</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>50000</v>
+      </c>
+      <c r="G12">
+        <v>17563749</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -10043,8 +10172,18 @@
         <f t="shared" si="1"/>
         <v>9.5445543828923476E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>50000</v>
+      </c>
+      <c r="G13">
+        <v>17563749</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -10062,8 +10201,18 @@
         <f t="shared" si="1"/>
         <v>1.5798762379740387E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>50000</v>
+      </c>
+      <c r="G14">
+        <v>17563749</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -10081,8 +10230,18 @@
         <f t="shared" si="1"/>
         <v>2.1252641283153713E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>50000</v>
+      </c>
+      <c r="G15">
+        <v>17563749</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -10100,8 +10259,18 @@
         <f t="shared" si="1"/>
         <v>1.3607740131341246E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>50000</v>
+      </c>
+      <c r="G16">
+        <v>17563749</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>278</v>
       </c>
@@ -10119,8 +10288,18 @@
         <f t="shared" si="1"/>
         <v>2.5950307568424636E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>50000</v>
+      </c>
+      <c r="G17">
+        <v>17563749</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -10138,8 +10317,18 @@
         <f t="shared" si="1"/>
         <v>2.2847303126557689E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>50000</v>
+      </c>
+      <c r="G18">
+        <v>17563749</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>287</v>
       </c>
@@ -10157,8 +10346,18 @@
         <f t="shared" si="1"/>
         <v>1.1935944528022361E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>50000</v>
+      </c>
+      <c r="G19">
+        <v>17563749</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -10176,8 +10375,18 @@
         <f t="shared" si="1"/>
         <v>1.669425901201602E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>50000</v>
+      </c>
+      <c r="G20">
+        <v>17563749</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>284</v>
       </c>
@@ -10195,8 +10404,18 @@
         <f t="shared" si="1"/>
         <v>7.0637044000144622E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>50000</v>
+      </c>
+      <c r="G21">
+        <v>17563749</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>292</v>
       </c>
@@ -10214,8 +10433,18 @@
         <f t="shared" si="1"/>
         <v>1.1302253942772849E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>50000</v>
+      </c>
+      <c r="G22">
+        <v>17563749</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>285</v>
       </c>
@@ -10233,8 +10462,18 @@
         <f t="shared" si="1"/>
         <v>5.4689550202067913E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>50000</v>
+      </c>
+      <c r="G23">
+        <v>17563749</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>275</v>
       </c>
@@ -10252,8 +10491,18 @@
         <f t="shared" si="1"/>
         <v>3.9479965748666955E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>50000</v>
+      </c>
+      <c r="G24">
+        <v>17563749</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -10271,8 +10520,18 @@
         <f t="shared" si="1"/>
         <v>5.2244892501871858E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>50000</v>
+      </c>
+      <c r="G25">
+        <v>17563749</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>276</v>
       </c>
@@ -10290,8 +10549,18 @@
         <f t="shared" si="1"/>
         <v>2.3695892105614243E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>50000</v>
+      </c>
+      <c r="G26">
+        <v>17563749</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>282</v>
       </c>
@@ -10309,8 +10578,18 @@
         <f t="shared" si="1"/>
         <v>4.9295263806931611E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>50000</v>
+      </c>
+      <c r="G27">
+        <v>17563749</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>281</v>
       </c>
@@ -10328,8 +10607,18 @@
         <f t="shared" si="1"/>
         <v>3.639538945162417E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>50000</v>
+      </c>
+      <c r="G28">
+        <v>17563749</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>288</v>
       </c>
@@ -10347,8 +10636,18 @@
         <f t="shared" si="1"/>
         <v>6.8205322895257044E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>50000</v>
+      </c>
+      <c r="G29">
+        <v>17563749</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>273</v>
       </c>
@@ -10366,8 +10665,18 @@
         <f t="shared" si="1"/>
         <v>3.2675092924368552E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>50000</v>
+      </c>
+      <c r="G30">
+        <v>17563749</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>125</v>
       </c>
@@ -10385,8 +10694,18 @@
         <f t="shared" si="1"/>
         <v>2.1664522853784571E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>50000</v>
+      </c>
+      <c r="G31">
+        <v>17563749</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>286</v>
       </c>
@@ -10404,8 +10723,18 @@
         <f t="shared" si="1"/>
         <v>2.0931428479598886E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>50000</v>
+      </c>
+      <c r="G32">
+        <v>17563749</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -10422,6 +10751,16 @@
       <c r="E33">
         <f t="shared" si="1"/>
         <v>1.4883871520668869E-2</v>
+      </c>
+      <c r="F33">
+        <v>50000</v>
+      </c>
+      <c r="G33">
+        <v>17563749</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>2.8467726337924777E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>